<commit_message>
JP-1480: support User parameter for Create Trigger
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Triggers.xlsx
+++ b/Workbooks/EN/Triggers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9320FC91-DDD6-4805-8794-6D3968AAD20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A83034E-CDE1-447A-80C8-C082D0246B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Get" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>Result</t>
   </si>
@@ -107,6 +107,14 @@
   </si>
   <si>
     <t>Items Per Job Activation Target</t>
+  </si>
+  <si>
+    <t>Username</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start Strategy (Execute XX times)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -330,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -368,11 +376,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="55">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -574,6 +583,17 @@
           <color theme="0" tint="-0.34998626667073579"/>
         </horizontal>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1731,60 +1751,61 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:V201" headerRowDxfId="53" dataDxfId="51" totalsRowDxfId="49" headerRowBorderDxfId="52" tableBorderDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:V201" headerRowDxfId="54" dataDxfId="52" totalsRowDxfId="50" headerRowBorderDxfId="53" tableBorderDxfId="51">
   <autoFilter ref="A1:V201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="22">
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Folder ID" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{058B7C0E-F18D-4AA8-A7A4-2A2B65B79498}" name="Folder Name" dataDxfId="47"/>
-    <tableColumn id="1" xr3:uid="{6FFDE20C-2159-4C8B-AE94-46A18EBF32E7}" name="Trigger ID" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{81F71C1A-632D-4A5F-BC94-CC97DF7A65EF}" name="Trigger Name" dataDxfId="45"/>
-    <tableColumn id="17" xr3:uid="{E6C314EE-6A01-4E6A-AF88-E0387E29802E}" name="Enabled" dataDxfId="44"/>
-    <tableColumn id="15" xr3:uid="{2DEE6F64-66B8-46E2-8DED-978C18789A63}" name="Process Name" dataDxfId="43"/>
-    <tableColumn id="14" xr3:uid="{6AFD31D0-7236-4B61-B6F7-B7E209179C91}" name="Input Arguments Definition" dataDxfId="42"/>
-    <tableColumn id="13" xr3:uid="{DB22136F-7CCB-43B3-B2F3-F64F00569B2B}" name="Use Calendar" dataDxfId="41"/>
-    <tableColumn id="12" xr3:uid="{4B4F4CCE-4592-4435-91E9-4E3F0FE0353D}" name="Start Strategy" dataDxfId="40"/>
-    <tableColumn id="11" xr3:uid="{6382E3E3-5FAD-4667-9BD7-D16BEF5953FF}" name="Start Process Cron" dataDxfId="39"/>
-    <tableColumn id="10" xr3:uid="{7A8F0FC9-8380-4F42-9505-29FB8CBCB859}" name="Start Process Cron Details" dataDxfId="38"/>
-    <tableColumn id="9" xr3:uid="{AF0F06BF-7B1B-43E6-A374-D2A97BE7CA57}" name="Stop Strategy" dataDxfId="37"/>
-    <tableColumn id="22" xr3:uid="{E47DF96B-8D93-4081-8137-B872BBA545F0}" name="Stop Process Date" dataDxfId="36"/>
-    <tableColumn id="21" xr3:uid="{5505F1C6-570D-45E3-9390-0F6EFEE4654C}" name="Stop Process Expression" dataDxfId="35"/>
-    <tableColumn id="20" xr3:uid="{5FBAB0A0-A21E-4CCD-980E-539376061F81}" name="Timezone" dataDxfId="34"/>
-    <tableColumn id="18" xr3:uid="{1EB4D3C2-CE07-4EA7-B2C8-74185C6E2FEF}" name="Job Priority" dataDxfId="33"/>
-    <tableColumn id="27" xr3:uid="{C533FEE6-8255-4711-A421-D6AB5A91A24C}" name="Items Activation Threshold" dataDxfId="32"/>
-    <tableColumn id="26" xr3:uid="{CC0987F9-E5EB-424C-BAC2-EC7C6CD6AE1A}" name="Items Per Job Activation" dataDxfId="31"/>
-    <tableColumn id="25" xr3:uid="{1AC94E67-3224-488F-8717-86F6A46274E7}" name="Max Jobs For Activation" dataDxfId="30"/>
-    <tableColumn id="23" xr3:uid="{30D62244-4112-4278-BA03-7537ABE2F931}" name="Queue Name" dataDxfId="29"/>
-    <tableColumn id="29" xr3:uid="{6F7B436B-C7DD-40F7-977E-79FB75EAFE78}" name="Calendar Name" dataDxfId="28"/>
-    <tableColumn id="28" xr3:uid="{E0816FFE-1BDE-49AC-A8E8-302C91411073}" name="Runtime Type" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Folder ID" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{058B7C0E-F18D-4AA8-A7A4-2A2B65B79498}" name="Folder Name" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{6FFDE20C-2159-4C8B-AE94-46A18EBF32E7}" name="Trigger ID" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{81F71C1A-632D-4A5F-BC94-CC97DF7A65EF}" name="Trigger Name" dataDxfId="46"/>
+    <tableColumn id="17" xr3:uid="{E6C314EE-6A01-4E6A-AF88-E0387E29802E}" name="Enabled" dataDxfId="45"/>
+    <tableColumn id="15" xr3:uid="{2DEE6F64-66B8-46E2-8DED-978C18789A63}" name="Process Name" dataDxfId="44"/>
+    <tableColumn id="14" xr3:uid="{6AFD31D0-7236-4B61-B6F7-B7E209179C91}" name="Input Arguments Definition" dataDxfId="43"/>
+    <tableColumn id="13" xr3:uid="{DB22136F-7CCB-43B3-B2F3-F64F00569B2B}" name="Use Calendar" dataDxfId="42"/>
+    <tableColumn id="12" xr3:uid="{4B4F4CCE-4592-4435-91E9-4E3F0FE0353D}" name="Start Strategy" dataDxfId="41"/>
+    <tableColumn id="11" xr3:uid="{6382E3E3-5FAD-4667-9BD7-D16BEF5953FF}" name="Start Process Cron" dataDxfId="40"/>
+    <tableColumn id="10" xr3:uid="{7A8F0FC9-8380-4F42-9505-29FB8CBCB859}" name="Start Process Cron Details" dataDxfId="39"/>
+    <tableColumn id="9" xr3:uid="{AF0F06BF-7B1B-43E6-A374-D2A97BE7CA57}" name="Stop Strategy" dataDxfId="38"/>
+    <tableColumn id="22" xr3:uid="{E47DF96B-8D93-4081-8137-B872BBA545F0}" name="Stop Process Date" dataDxfId="37"/>
+    <tableColumn id="21" xr3:uid="{5505F1C6-570D-45E3-9390-0F6EFEE4654C}" name="Stop Process Expression" dataDxfId="36"/>
+    <tableColumn id="20" xr3:uid="{5FBAB0A0-A21E-4CCD-980E-539376061F81}" name="Timezone" dataDxfId="35"/>
+    <tableColumn id="18" xr3:uid="{1EB4D3C2-CE07-4EA7-B2C8-74185C6E2FEF}" name="Job Priority" dataDxfId="34"/>
+    <tableColumn id="27" xr3:uid="{C533FEE6-8255-4711-A421-D6AB5A91A24C}" name="Items Activation Threshold" dataDxfId="33"/>
+    <tableColumn id="26" xr3:uid="{CC0987F9-E5EB-424C-BAC2-EC7C6CD6AE1A}" name="Items Per Job Activation" dataDxfId="32"/>
+    <tableColumn id="25" xr3:uid="{1AC94E67-3224-488F-8717-86F6A46274E7}" name="Max Jobs For Activation" dataDxfId="31"/>
+    <tableColumn id="23" xr3:uid="{30D62244-4112-4278-BA03-7537ABE2F931}" name="Queue Name" dataDxfId="30"/>
+    <tableColumn id="29" xr3:uid="{6F7B436B-C7DD-40F7-977E-79FB75EAFE78}" name="Calendar Name" dataDxfId="29"/>
+    <tableColumn id="28" xr3:uid="{E0816FFE-1BDE-49AC-A8E8-302C91411073}" name="Runtime Type" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:V201" totalsRowShown="0">
-  <autoFilter ref="A1:V201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="22">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Folder Name" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{3F114B58-2997-4D73-A80A-40D21B742757}" name="Trigger Name" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{45B7C249-3DF1-450D-AA47-E72B0FE30A90}" name="Enabled" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{FD574CB7-FA08-4654-9CD7-86D60F34DB32}" name="Process Name" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{7446F334-E6E0-4A0E-8EB5-68FB9D43F164}" name="Input Arguments Definition" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{9112BA16-F1A6-4B5B-9292-E1F862C46582}" name="Use Calendar" dataDxfId="21"/>
-    <tableColumn id="17" xr3:uid="{EDBD2CF6-8937-4430-880E-CBC035D999B9}" name="Start Strategy" dataDxfId="20"/>
-    <tableColumn id="16" xr3:uid="{17E46FA8-B1FA-4C01-B909-101B4EBE2771}" name="Start Process Cron" dataDxfId="19"/>
-    <tableColumn id="15" xr3:uid="{C32A3E10-03CD-4CDE-862C-B8BCCE543C7C}" name="Start Process Cron Details" dataDxfId="18"/>
-    <tableColumn id="14" xr3:uid="{DF244F76-D9C5-4B2A-A7FF-45B1E3C0C680}" name="Stop Strategy" dataDxfId="17"/>
-    <tableColumn id="13" xr3:uid="{F8BF873D-C98E-4452-A769-1730BAA59018}" name="Stop Process Date" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{F1B1C282-F479-4190-ADF0-BBDE31D5EFDB}" name="Stop Process Expression" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{670C436B-1C2B-4D6A-86BB-6E37C846E72C}" name="Timezone" dataDxfId="14"/>
-    <tableColumn id="21" xr3:uid="{95C00957-7AEE-4E5A-8494-3D628AFB4D6C}" name="Job Priority" dataDxfId="13"/>
-    <tableColumn id="20" xr3:uid="{CDA69AC6-5479-479E-B18C-36DFF3254945}" name="Items Activation Threshold" dataDxfId="12"/>
-    <tableColumn id="19" xr3:uid="{8E859498-36EB-4FDD-AAD6-41CC93FE4779}" name="Items Per Job Activation Target" dataDxfId="11"/>
-    <tableColumn id="18" xr3:uid="{08F82746-079C-4356-9DB9-1968920B347F}" name="Max Jobs For Activation" dataDxfId="10"/>
-    <tableColumn id="25" xr3:uid="{3EFAE5F4-8E3E-477D-95CB-475B3BAF404F}" name="Queue Name" dataDxfId="9"/>
-    <tableColumn id="24" xr3:uid="{FE42FDBB-617A-49AC-9EEA-7F486125AE50}" name="Calendar Name" dataDxfId="8"/>
-    <tableColumn id="23" xr3:uid="{FF130F51-8B1A-4457-8500-568BE985E460}" name="Runtime Type" dataDxfId="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:W201" totalsRowShown="0">
+  <autoFilter ref="A1:W201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="23">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Folder Name" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{3F114B58-2997-4D73-A80A-40D21B742757}" name="Trigger Name" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{45B7C249-3DF1-450D-AA47-E72B0FE30A90}" name="Enabled" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{FD574CB7-FA08-4654-9CD7-86D60F34DB32}" name="Process Name" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{7446F334-E6E0-4A0E-8EB5-68FB9D43F164}" name="Input Arguments Definition" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{9112BA16-F1A6-4B5B-9292-E1F862C46582}" name="Use Calendar" dataDxfId="22"/>
+    <tableColumn id="17" xr3:uid="{EDBD2CF6-8937-4430-880E-CBC035D999B9}" name="Start Strategy (Execute XX times)" dataDxfId="21"/>
+    <tableColumn id="16" xr3:uid="{17E46FA8-B1FA-4C01-B909-101B4EBE2771}" name="Start Process Cron" dataDxfId="20"/>
+    <tableColumn id="15" xr3:uid="{C32A3E10-03CD-4CDE-862C-B8BCCE543C7C}" name="Start Process Cron Details" dataDxfId="19"/>
+    <tableColumn id="14" xr3:uid="{DF244F76-D9C5-4B2A-A7FF-45B1E3C0C680}" name="Stop Strategy" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{F8BF873D-C98E-4452-A769-1730BAA59018}" name="Stop Process Date" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{F1B1C282-F479-4190-ADF0-BBDE31D5EFDB}" name="Stop Process Expression" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{670C436B-1C2B-4D6A-86BB-6E37C846E72C}" name="Timezone" dataDxfId="15"/>
+    <tableColumn id="21" xr3:uid="{95C00957-7AEE-4E5A-8494-3D628AFB4D6C}" name="Job Priority" dataDxfId="14"/>
+    <tableColumn id="20" xr3:uid="{CDA69AC6-5479-479E-B18C-36DFF3254945}" name="Items Activation Threshold" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{8E859498-36EB-4FDD-AAD6-41CC93FE4779}" name="Items Per Job Activation Target" dataDxfId="12"/>
+    <tableColumn id="18" xr3:uid="{08F82746-079C-4356-9DB9-1968920B347F}" name="Max Jobs For Activation" dataDxfId="11"/>
+    <tableColumn id="25" xr3:uid="{3EFAE5F4-8E3E-477D-95CB-475B3BAF404F}" name="Queue Name" dataDxfId="10"/>
+    <tableColumn id="24" xr3:uid="{FE42FDBB-617A-49AC-9EEA-7F486125AE50}" name="Calendar Name" dataDxfId="9"/>
+    <tableColumn id="23" xr3:uid="{FF130F51-8B1A-4457-8500-568BE985E460}" name="Runtime Type" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{4F583ADB-8987-4584-9B76-C3EFCC339400}" name="Username" dataDxfId="7"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Trigger ID" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="Result" dataDxfId="5"/>
   </tableColumns>
@@ -2071,7 +2092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B90804-4CC2-4F3A-A5A0-B313E9BACDDF}">
   <dimension ref="A1:V201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6996,10 +7017,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V201"/>
+  <dimension ref="A1:W201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -7008,19 +7029,20 @@
     <col min="3" max="3" width="15.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.5" style="20" customWidth="1"/>
     <col min="5" max="5" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="36.25" customWidth="1"/>
     <col min="8" max="8" width="25.5" customWidth="1"/>
     <col min="9" max="9" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="13" width="25.5" customWidth="1"/>
     <col min="14" max="14" width="15.5" customWidth="1"/>
     <col min="15" max="15" width="27.4140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="25.5" customWidth="1"/>
-    <col min="21" max="21" width="15.5" customWidth="1"/>
-    <col min="22" max="22" width="45.5" customWidth="1"/>
+    <col min="17" max="21" width="25.5" customWidth="1"/>
+    <col min="22" max="22" width="15.5" customWidth="1"/>
+    <col min="23" max="23" width="45.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
         <v>21</v>
       </c>
@@ -7040,7 +7062,7 @@
         <v>6</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>8</v>
@@ -7081,14 +7103,17 @@
       <c r="T1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="U1" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="11"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -7109,10 +7134,11 @@
       <c r="R2" s="13"/>
       <c r="S2" s="13"/>
       <c r="T2" s="13"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="5"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U2" s="23"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="5"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -7133,10 +7159,11 @@
       <c r="R3" s="13"/>
       <c r="S3" s="13"/>
       <c r="T3" s="13"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="5"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U3" s="23"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="5"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="11"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -7157,10 +7184,11 @@
       <c r="R4" s="13"/>
       <c r="S4" s="13"/>
       <c r="T4" s="13"/>
-      <c r="U4" s="5"/>
+      <c r="U4" s="23"/>
       <c r="V4" s="5"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W4" s="5"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="11"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -7181,10 +7209,11 @@
       <c r="R5" s="13"/>
       <c r="S5" s="13"/>
       <c r="T5" s="13"/>
-      <c r="U5" s="5"/>
+      <c r="U5" s="23"/>
       <c r="V5" s="5"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W5" s="5"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="11"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -7205,10 +7234,11 @@
       <c r="R6" s="13"/>
       <c r="S6" s="13"/>
       <c r="T6" s="13"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="5"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U6" s="23"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="5"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="11"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -7229,10 +7259,11 @@
       <c r="R7" s="13"/>
       <c r="S7" s="13"/>
       <c r="T7" s="13"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="5"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U7" s="23"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="5"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="11"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -7253,10 +7284,11 @@
       <c r="R8" s="13"/>
       <c r="S8" s="13"/>
       <c r="T8" s="13"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="5"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U8" s="23"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="5"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="11"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -7277,10 +7309,11 @@
       <c r="R9" s="13"/>
       <c r="S9" s="13"/>
       <c r="T9" s="13"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="5"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U9" s="23"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="5"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="11"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -7301,10 +7334,11 @@
       <c r="R10" s="13"/>
       <c r="S10" s="13"/>
       <c r="T10" s="13"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="5"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U10" s="23"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="5"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="11"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -7325,10 +7359,11 @@
       <c r="R11" s="13"/>
       <c r="S11" s="13"/>
       <c r="T11" s="13"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="5"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U11" s="23"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="5"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="11"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -7349,10 +7384,11 @@
       <c r="R12" s="13"/>
       <c r="S12" s="13"/>
       <c r="T12" s="13"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="5"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U12" s="23"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="5"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="11"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -7373,10 +7409,11 @@
       <c r="R13" s="13"/>
       <c r="S13" s="13"/>
       <c r="T13" s="13"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="5"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U13" s="23"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="5"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="11"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -7397,10 +7434,11 @@
       <c r="R14" s="13"/>
       <c r="S14" s="13"/>
       <c r="T14" s="13"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="5"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U14" s="23"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="5"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="11"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -7421,10 +7459,11 @@
       <c r="R15" s="13"/>
       <c r="S15" s="13"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="5"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U15" s="23"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="5"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="11"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -7445,10 +7484,11 @@
       <c r="R16" s="13"/>
       <c r="S16" s="13"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="5"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U16" s="23"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="5"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="11"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -7469,10 +7509,11 @@
       <c r="R17" s="13"/>
       <c r="S17" s="13"/>
       <c r="T17" s="13"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="5"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U17" s="23"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="5"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="11"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -7493,10 +7534,11 @@
       <c r="R18" s="13"/>
       <c r="S18" s="13"/>
       <c r="T18" s="13"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="5"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U18" s="23"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="5"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="11"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -7517,10 +7559,11 @@
       <c r="R19" s="13"/>
       <c r="S19" s="13"/>
       <c r="T19" s="13"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="5"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U19" s="23"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="5"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="11"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -7541,10 +7584,11 @@
       <c r="R20" s="13"/>
       <c r="S20" s="13"/>
       <c r="T20" s="13"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="5"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U20" s="23"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="5"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="11"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
@@ -7565,10 +7609,11 @@
       <c r="R21" s="13"/>
       <c r="S21" s="13"/>
       <c r="T21" s="13"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="5"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U21" s="23"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="5"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="11"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -7589,10 +7634,11 @@
       <c r="R22" s="13"/>
       <c r="S22" s="13"/>
       <c r="T22" s="13"/>
-      <c r="U22" s="8"/>
-      <c r="V22" s="5"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U22" s="23"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="5"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="11"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -7613,10 +7659,11 @@
       <c r="R23" s="13"/>
       <c r="S23" s="13"/>
       <c r="T23" s="13"/>
-      <c r="U23" s="8"/>
-      <c r="V23" s="5"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U23" s="23"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="5"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="11"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
@@ -7637,10 +7684,11 @@
       <c r="R24" s="13"/>
       <c r="S24" s="13"/>
       <c r="T24" s="13"/>
-      <c r="U24" s="8"/>
-      <c r="V24" s="5"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U24" s="23"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="5"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="11"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -7661,10 +7709,11 @@
       <c r="R25" s="13"/>
       <c r="S25" s="13"/>
       <c r="T25" s="13"/>
-      <c r="U25" s="8"/>
-      <c r="V25" s="5"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U25" s="23"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="5"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="11"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -7685,10 +7734,11 @@
       <c r="R26" s="13"/>
       <c r="S26" s="13"/>
       <c r="T26" s="13"/>
-      <c r="U26" s="8"/>
-      <c r="V26" s="5"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U26" s="23"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="5"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="11"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -7709,10 +7759,11 @@
       <c r="R27" s="13"/>
       <c r="S27" s="13"/>
       <c r="T27" s="13"/>
-      <c r="U27" s="8"/>
-      <c r="V27" s="5"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U27" s="23"/>
+      <c r="V27" s="8"/>
+      <c r="W27" s="5"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="11"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -7733,10 +7784,11 @@
       <c r="R28" s="13"/>
       <c r="S28" s="13"/>
       <c r="T28" s="13"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="5"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U28" s="23"/>
+      <c r="V28" s="8"/>
+      <c r="W28" s="5"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="11"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -7757,10 +7809,11 @@
       <c r="R29" s="13"/>
       <c r="S29" s="13"/>
       <c r="T29" s="13"/>
-      <c r="U29" s="8"/>
-      <c r="V29" s="5"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U29" s="23"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="5"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="11"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -7781,10 +7834,11 @@
       <c r="R30" s="13"/>
       <c r="S30" s="13"/>
       <c r="T30" s="13"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="5"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U30" s="23"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="5"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="11"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -7805,10 +7859,11 @@
       <c r="R31" s="13"/>
       <c r="S31" s="13"/>
       <c r="T31" s="13"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="5"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U31" s="23"/>
+      <c r="V31" s="8"/>
+      <c r="W31" s="5"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="11"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -7829,10 +7884,11 @@
       <c r="R32" s="13"/>
       <c r="S32" s="13"/>
       <c r="T32" s="13"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="5"/>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U32" s="23"/>
+      <c r="V32" s="8"/>
+      <c r="W32" s="5"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="11"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -7853,10 +7909,11 @@
       <c r="R33" s="13"/>
       <c r="S33" s="13"/>
       <c r="T33" s="13"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="5"/>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U33" s="23"/>
+      <c r="V33" s="8"/>
+      <c r="W33" s="5"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="11"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -7877,10 +7934,11 @@
       <c r="R34" s="13"/>
       <c r="S34" s="13"/>
       <c r="T34" s="13"/>
-      <c r="U34" s="8"/>
-      <c r="V34" s="5"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U34" s="23"/>
+      <c r="V34" s="8"/>
+      <c r="W34" s="5"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="11"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -7901,10 +7959,11 @@
       <c r="R35" s="13"/>
       <c r="S35" s="13"/>
       <c r="T35" s="13"/>
-      <c r="U35" s="8"/>
-      <c r="V35" s="5"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U35" s="23"/>
+      <c r="V35" s="8"/>
+      <c r="W35" s="5"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="11"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -7925,10 +7984,11 @@
       <c r="R36" s="13"/>
       <c r="S36" s="13"/>
       <c r="T36" s="13"/>
-      <c r="U36" s="8"/>
-      <c r="V36" s="5"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U36" s="23"/>
+      <c r="V36" s="8"/>
+      <c r="W36" s="5"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="11"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -7949,10 +8009,11 @@
       <c r="R37" s="13"/>
       <c r="S37" s="13"/>
       <c r="T37" s="13"/>
-      <c r="U37" s="8"/>
-      <c r="V37" s="5"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U37" s="23"/>
+      <c r="V37" s="8"/>
+      <c r="W37" s="5"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="11"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -7973,10 +8034,11 @@
       <c r="R38" s="13"/>
       <c r="S38" s="13"/>
       <c r="T38" s="13"/>
-      <c r="U38" s="8"/>
-      <c r="V38" s="5"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U38" s="23"/>
+      <c r="V38" s="8"/>
+      <c r="W38" s="5"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="11"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -7997,10 +8059,11 @@
       <c r="R39" s="13"/>
       <c r="S39" s="13"/>
       <c r="T39" s="13"/>
-      <c r="U39" s="8"/>
-      <c r="V39" s="5"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U39" s="23"/>
+      <c r="V39" s="8"/>
+      <c r="W39" s="5"/>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="11"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -8021,10 +8084,11 @@
       <c r="R40" s="13"/>
       <c r="S40" s="13"/>
       <c r="T40" s="13"/>
-      <c r="U40" s="8"/>
-      <c r="V40" s="5"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U40" s="23"/>
+      <c r="V40" s="8"/>
+      <c r="W40" s="5"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="11"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -8045,10 +8109,11 @@
       <c r="R41" s="13"/>
       <c r="S41" s="13"/>
       <c r="T41" s="13"/>
-      <c r="U41" s="8"/>
-      <c r="V41" s="5"/>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U41" s="23"/>
+      <c r="V41" s="8"/>
+      <c r="W41" s="5"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="11"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
@@ -8069,10 +8134,11 @@
       <c r="R42" s="13"/>
       <c r="S42" s="13"/>
       <c r="T42" s="13"/>
-      <c r="U42" s="8"/>
-      <c r="V42" s="5"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U42" s="23"/>
+      <c r="V42" s="8"/>
+      <c r="W42" s="5"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="11"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
@@ -8093,10 +8159,11 @@
       <c r="R43" s="13"/>
       <c r="S43" s="13"/>
       <c r="T43" s="13"/>
-      <c r="U43" s="8"/>
-      <c r="V43" s="5"/>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U43" s="23"/>
+      <c r="V43" s="8"/>
+      <c r="W43" s="5"/>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="11"/>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
@@ -8117,10 +8184,11 @@
       <c r="R44" s="13"/>
       <c r="S44" s="13"/>
       <c r="T44" s="13"/>
-      <c r="U44" s="8"/>
-      <c r="V44" s="5"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U44" s="23"/>
+      <c r="V44" s="8"/>
+      <c r="W44" s="5"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="11"/>
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
@@ -8141,10 +8209,11 @@
       <c r="R45" s="13"/>
       <c r="S45" s="13"/>
       <c r="T45" s="13"/>
-      <c r="U45" s="8"/>
-      <c r="V45" s="5"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U45" s="23"/>
+      <c r="V45" s="8"/>
+      <c r="W45" s="5"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="11"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
@@ -8165,10 +8234,11 @@
       <c r="R46" s="13"/>
       <c r="S46" s="13"/>
       <c r="T46" s="13"/>
-      <c r="U46" s="8"/>
-      <c r="V46" s="5"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U46" s="23"/>
+      <c r="V46" s="8"/>
+      <c r="W46" s="5"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="11"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
@@ -8189,10 +8259,11 @@
       <c r="R47" s="13"/>
       <c r="S47" s="13"/>
       <c r="T47" s="13"/>
-      <c r="U47" s="8"/>
-      <c r="V47" s="5"/>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U47" s="23"/>
+      <c r="V47" s="8"/>
+      <c r="W47" s="5"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="11"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
@@ -8213,10 +8284,11 @@
       <c r="R48" s="13"/>
       <c r="S48" s="13"/>
       <c r="T48" s="13"/>
-      <c r="U48" s="8"/>
-      <c r="V48" s="5"/>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U48" s="23"/>
+      <c r="V48" s="8"/>
+      <c r="W48" s="5"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="11"/>
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
@@ -8237,10 +8309,11 @@
       <c r="R49" s="13"/>
       <c r="S49" s="13"/>
       <c r="T49" s="13"/>
-      <c r="U49" s="8"/>
-      <c r="V49" s="5"/>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U49" s="23"/>
+      <c r="V49" s="8"/>
+      <c r="W49" s="5"/>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="11"/>
       <c r="B50" s="13"/>
       <c r="C50" s="13"/>
@@ -8261,10 +8334,11 @@
       <c r="R50" s="13"/>
       <c r="S50" s="13"/>
       <c r="T50" s="13"/>
-      <c r="U50" s="8"/>
-      <c r="V50" s="5"/>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U50" s="23"/>
+      <c r="V50" s="8"/>
+      <c r="W50" s="5"/>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="11"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
@@ -8285,10 +8359,11 @@
       <c r="R51" s="13"/>
       <c r="S51" s="13"/>
       <c r="T51" s="13"/>
-      <c r="U51" s="8"/>
-      <c r="V51" s="5"/>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U51" s="23"/>
+      <c r="V51" s="8"/>
+      <c r="W51" s="5"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="11"/>
       <c r="B52" s="13"/>
       <c r="C52" s="13"/>
@@ -8309,10 +8384,11 @@
       <c r="R52" s="13"/>
       <c r="S52" s="13"/>
       <c r="T52" s="13"/>
-      <c r="U52" s="8"/>
-      <c r="V52" s="5"/>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U52" s="23"/>
+      <c r="V52" s="8"/>
+      <c r="W52" s="5"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="11"/>
       <c r="B53" s="13"/>
       <c r="C53" s="13"/>
@@ -8333,10 +8409,11 @@
       <c r="R53" s="13"/>
       <c r="S53" s="13"/>
       <c r="T53" s="13"/>
-      <c r="U53" s="8"/>
-      <c r="V53" s="5"/>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U53" s="23"/>
+      <c r="V53" s="8"/>
+      <c r="W53" s="5"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="11"/>
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
@@ -8357,10 +8434,11 @@
       <c r="R54" s="13"/>
       <c r="S54" s="13"/>
       <c r="T54" s="13"/>
-      <c r="U54" s="8"/>
-      <c r="V54" s="5"/>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U54" s="23"/>
+      <c r="V54" s="8"/>
+      <c r="W54" s="5"/>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="11"/>
       <c r="B55" s="13"/>
       <c r="C55" s="13"/>
@@ -8381,10 +8459,11 @@
       <c r="R55" s="13"/>
       <c r="S55" s="13"/>
       <c r="T55" s="13"/>
-      <c r="U55" s="8"/>
-      <c r="V55" s="5"/>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U55" s="23"/>
+      <c r="V55" s="8"/>
+      <c r="W55" s="5"/>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="11"/>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
@@ -8405,10 +8484,11 @@
       <c r="R56" s="13"/>
       <c r="S56" s="13"/>
       <c r="T56" s="13"/>
-      <c r="U56" s="8"/>
-      <c r="V56" s="5"/>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U56" s="23"/>
+      <c r="V56" s="8"/>
+      <c r="W56" s="5"/>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="11"/>
       <c r="B57" s="13"/>
       <c r="C57" s="13"/>
@@ -8429,10 +8509,11 @@
       <c r="R57" s="13"/>
       <c r="S57" s="13"/>
       <c r="T57" s="13"/>
-      <c r="U57" s="8"/>
-      <c r="V57" s="5"/>
-    </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U57" s="23"/>
+      <c r="V57" s="8"/>
+      <c r="W57" s="5"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="11"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
@@ -8453,10 +8534,11 @@
       <c r="R58" s="13"/>
       <c r="S58" s="13"/>
       <c r="T58" s="13"/>
-      <c r="U58" s="8"/>
-      <c r="V58" s="5"/>
-    </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U58" s="23"/>
+      <c r="V58" s="8"/>
+      <c r="W58" s="5"/>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="11"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
@@ -8477,10 +8559,11 @@
       <c r="R59" s="13"/>
       <c r="S59" s="13"/>
       <c r="T59" s="13"/>
-      <c r="U59" s="8"/>
-      <c r="V59" s="5"/>
-    </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U59" s="23"/>
+      <c r="V59" s="8"/>
+      <c r="W59" s="5"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="11"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
@@ -8501,10 +8584,11 @@
       <c r="R60" s="13"/>
       <c r="S60" s="13"/>
       <c r="T60" s="13"/>
-      <c r="U60" s="8"/>
-      <c r="V60" s="5"/>
-    </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U60" s="23"/>
+      <c r="V60" s="8"/>
+      <c r="W60" s="5"/>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="11"/>
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
@@ -8525,10 +8609,11 @@
       <c r="R61" s="13"/>
       <c r="S61" s="13"/>
       <c r="T61" s="13"/>
-      <c r="U61" s="8"/>
-      <c r="V61" s="5"/>
-    </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U61" s="23"/>
+      <c r="V61" s="8"/>
+      <c r="W61" s="5"/>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="11"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -8549,10 +8634,11 @@
       <c r="R62" s="13"/>
       <c r="S62" s="13"/>
       <c r="T62" s="13"/>
-      <c r="U62" s="8"/>
-      <c r="V62" s="5"/>
-    </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U62" s="23"/>
+      <c r="V62" s="8"/>
+      <c r="W62" s="5"/>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="11"/>
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
@@ -8573,10 +8659,11 @@
       <c r="R63" s="13"/>
       <c r="S63" s="13"/>
       <c r="T63" s="13"/>
-      <c r="U63" s="8"/>
-      <c r="V63" s="5"/>
-    </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U63" s="23"/>
+      <c r="V63" s="8"/>
+      <c r="W63" s="5"/>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="11"/>
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
@@ -8597,10 +8684,11 @@
       <c r="R64" s="13"/>
       <c r="S64" s="13"/>
       <c r="T64" s="13"/>
-      <c r="U64" s="8"/>
-      <c r="V64" s="5"/>
-    </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U64" s="23"/>
+      <c r="V64" s="8"/>
+      <c r="W64" s="5"/>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="11"/>
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
@@ -8621,10 +8709,11 @@
       <c r="R65" s="13"/>
       <c r="S65" s="13"/>
       <c r="T65" s="13"/>
-      <c r="U65" s="8"/>
-      <c r="V65" s="5"/>
-    </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U65" s="23"/>
+      <c r="V65" s="8"/>
+      <c r="W65" s="5"/>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="11"/>
       <c r="B66" s="13"/>
       <c r="C66" s="13"/>
@@ -8645,10 +8734,11 @@
       <c r="R66" s="13"/>
       <c r="S66" s="13"/>
       <c r="T66" s="13"/>
-      <c r="U66" s="8"/>
-      <c r="V66" s="5"/>
-    </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U66" s="23"/>
+      <c r="V66" s="8"/>
+      <c r="W66" s="5"/>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="11"/>
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
@@ -8669,10 +8759,11 @@
       <c r="R67" s="13"/>
       <c r="S67" s="13"/>
       <c r="T67" s="13"/>
-      <c r="U67" s="8"/>
-      <c r="V67" s="5"/>
-    </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U67" s="23"/>
+      <c r="V67" s="8"/>
+      <c r="W67" s="5"/>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="11"/>
       <c r="B68" s="13"/>
       <c r="C68" s="13"/>
@@ -8693,10 +8784,11 @@
       <c r="R68" s="13"/>
       <c r="S68" s="13"/>
       <c r="T68" s="13"/>
-      <c r="U68" s="8"/>
-      <c r="V68" s="5"/>
-    </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U68" s="23"/>
+      <c r="V68" s="8"/>
+      <c r="W68" s="5"/>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="11"/>
       <c r="B69" s="13"/>
       <c r="C69" s="13"/>
@@ -8717,10 +8809,11 @@
       <c r="R69" s="13"/>
       <c r="S69" s="13"/>
       <c r="T69" s="13"/>
-      <c r="U69" s="8"/>
-      <c r="V69" s="5"/>
-    </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U69" s="23"/>
+      <c r="V69" s="8"/>
+      <c r="W69" s="5"/>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="11"/>
       <c r="B70" s="13"/>
       <c r="C70" s="13"/>
@@ -8741,10 +8834,11 @@
       <c r="R70" s="13"/>
       <c r="S70" s="13"/>
       <c r="T70" s="13"/>
-      <c r="U70" s="8"/>
-      <c r="V70" s="5"/>
-    </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U70" s="23"/>
+      <c r="V70" s="8"/>
+      <c r="W70" s="5"/>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="11"/>
       <c r="B71" s="13"/>
       <c r="C71" s="13"/>
@@ -8765,10 +8859,11 @@
       <c r="R71" s="13"/>
       <c r="S71" s="13"/>
       <c r="T71" s="13"/>
-      <c r="U71" s="8"/>
-      <c r="V71" s="5"/>
-    </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U71" s="23"/>
+      <c r="V71" s="8"/>
+      <c r="W71" s="5"/>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="11"/>
       <c r="B72" s="13"/>
       <c r="C72" s="13"/>
@@ -8789,10 +8884,11 @@
       <c r="R72" s="13"/>
       <c r="S72" s="13"/>
       <c r="T72" s="13"/>
-      <c r="U72" s="8"/>
-      <c r="V72" s="5"/>
-    </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U72" s="23"/>
+      <c r="V72" s="8"/>
+      <c r="W72" s="5"/>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="11"/>
       <c r="B73" s="13"/>
       <c r="C73" s="13"/>
@@ -8813,10 +8909,11 @@
       <c r="R73" s="13"/>
       <c r="S73" s="13"/>
       <c r="T73" s="13"/>
-      <c r="U73" s="8"/>
-      <c r="V73" s="5"/>
-    </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U73" s="23"/>
+      <c r="V73" s="8"/>
+      <c r="W73" s="5"/>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="11"/>
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
@@ -8837,10 +8934,11 @@
       <c r="R74" s="13"/>
       <c r="S74" s="13"/>
       <c r="T74" s="13"/>
-      <c r="U74" s="8"/>
-      <c r="V74" s="5"/>
-    </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U74" s="23"/>
+      <c r="V74" s="8"/>
+      <c r="W74" s="5"/>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="11"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
@@ -8861,10 +8959,11 @@
       <c r="R75" s="13"/>
       <c r="S75" s="13"/>
       <c r="T75" s="13"/>
-      <c r="U75" s="8"/>
-      <c r="V75" s="5"/>
-    </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U75" s="23"/>
+      <c r="V75" s="8"/>
+      <c r="W75" s="5"/>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="11"/>
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
@@ -8885,10 +8984,11 @@
       <c r="R76" s="13"/>
       <c r="S76" s="13"/>
       <c r="T76" s="13"/>
-      <c r="U76" s="8"/>
-      <c r="V76" s="5"/>
-    </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U76" s="23"/>
+      <c r="V76" s="8"/>
+      <c r="W76" s="5"/>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="11"/>
       <c r="B77" s="13"/>
       <c r="C77" s="13"/>
@@ -8909,10 +9009,11 @@
       <c r="R77" s="13"/>
       <c r="S77" s="13"/>
       <c r="T77" s="13"/>
-      <c r="U77" s="8"/>
-      <c r="V77" s="5"/>
-    </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U77" s="23"/>
+      <c r="V77" s="8"/>
+      <c r="W77" s="5"/>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="11"/>
       <c r="B78" s="13"/>
       <c r="C78" s="13"/>
@@ -8933,10 +9034,11 @@
       <c r="R78" s="13"/>
       <c r="S78" s="13"/>
       <c r="T78" s="13"/>
-      <c r="U78" s="8"/>
-      <c r="V78" s="5"/>
-    </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U78" s="23"/>
+      <c r="V78" s="8"/>
+      <c r="W78" s="5"/>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="11"/>
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
@@ -8957,10 +9059,11 @@
       <c r="R79" s="13"/>
       <c r="S79" s="13"/>
       <c r="T79" s="13"/>
-      <c r="U79" s="8"/>
-      <c r="V79" s="5"/>
-    </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U79" s="23"/>
+      <c r="V79" s="8"/>
+      <c r="W79" s="5"/>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="11"/>
       <c r="B80" s="13"/>
       <c r="C80" s="13"/>
@@ -8981,10 +9084,11 @@
       <c r="R80" s="13"/>
       <c r="S80" s="13"/>
       <c r="T80" s="13"/>
-      <c r="U80" s="8"/>
-      <c r="V80" s="5"/>
-    </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U80" s="23"/>
+      <c r="V80" s="8"/>
+      <c r="W80" s="5"/>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="11"/>
       <c r="B81" s="13"/>
       <c r="C81" s="13"/>
@@ -9005,10 +9109,11 @@
       <c r="R81" s="13"/>
       <c r="S81" s="13"/>
       <c r="T81" s="13"/>
-      <c r="U81" s="8"/>
-      <c r="V81" s="5"/>
-    </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U81" s="23"/>
+      <c r="V81" s="8"/>
+      <c r="W81" s="5"/>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="11"/>
       <c r="B82" s="13"/>
       <c r="C82" s="13"/>
@@ -9029,10 +9134,11 @@
       <c r="R82" s="13"/>
       <c r="S82" s="13"/>
       <c r="T82" s="13"/>
-      <c r="U82" s="8"/>
-      <c r="V82" s="5"/>
-    </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U82" s="23"/>
+      <c r="V82" s="8"/>
+      <c r="W82" s="5"/>
+    </row>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="11"/>
       <c r="B83" s="13"/>
       <c r="C83" s="13"/>
@@ -9053,10 +9159,11 @@
       <c r="R83" s="13"/>
       <c r="S83" s="13"/>
       <c r="T83" s="13"/>
-      <c r="U83" s="8"/>
-      <c r="V83" s="5"/>
-    </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U83" s="23"/>
+      <c r="V83" s="8"/>
+      <c r="W83" s="5"/>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="11"/>
       <c r="B84" s="13"/>
       <c r="C84" s="13"/>
@@ -9077,10 +9184,11 @@
       <c r="R84" s="13"/>
       <c r="S84" s="13"/>
       <c r="T84" s="13"/>
-      <c r="U84" s="8"/>
-      <c r="V84" s="5"/>
-    </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U84" s="23"/>
+      <c r="V84" s="8"/>
+      <c r="W84" s="5"/>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="11"/>
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
@@ -9101,10 +9209,11 @@
       <c r="R85" s="13"/>
       <c r="S85" s="13"/>
       <c r="T85" s="13"/>
-      <c r="U85" s="8"/>
-      <c r="V85" s="5"/>
-    </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U85" s="23"/>
+      <c r="V85" s="8"/>
+      <c r="W85" s="5"/>
+    </row>
+    <row r="86" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="11"/>
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
@@ -9125,10 +9234,11 @@
       <c r="R86" s="13"/>
       <c r="S86" s="13"/>
       <c r="T86" s="13"/>
-      <c r="U86" s="8"/>
-      <c r="V86" s="5"/>
-    </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U86" s="23"/>
+      <c r="V86" s="8"/>
+      <c r="W86" s="5"/>
+    </row>
+    <row r="87" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="11"/>
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
@@ -9149,10 +9259,11 @@
       <c r="R87" s="13"/>
       <c r="S87" s="13"/>
       <c r="T87" s="13"/>
-      <c r="U87" s="8"/>
-      <c r="V87" s="5"/>
-    </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U87" s="23"/>
+      <c r="V87" s="8"/>
+      <c r="W87" s="5"/>
+    </row>
+    <row r="88" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="11"/>
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
@@ -9173,10 +9284,11 @@
       <c r="R88" s="13"/>
       <c r="S88" s="13"/>
       <c r="T88" s="13"/>
-      <c r="U88" s="8"/>
-      <c r="V88" s="5"/>
-    </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U88" s="23"/>
+      <c r="V88" s="8"/>
+      <c r="W88" s="5"/>
+    </row>
+    <row r="89" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="11"/>
       <c r="B89" s="13"/>
       <c r="C89" s="13"/>
@@ -9197,10 +9309,11 @@
       <c r="R89" s="13"/>
       <c r="S89" s="13"/>
       <c r="T89" s="13"/>
-      <c r="U89" s="8"/>
-      <c r="V89" s="5"/>
-    </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U89" s="23"/>
+      <c r="V89" s="8"/>
+      <c r="W89" s="5"/>
+    </row>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="11"/>
       <c r="B90" s="13"/>
       <c r="C90" s="13"/>
@@ -9221,10 +9334,11 @@
       <c r="R90" s="13"/>
       <c r="S90" s="13"/>
       <c r="T90" s="13"/>
-      <c r="U90" s="8"/>
-      <c r="V90" s="5"/>
-    </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U90" s="23"/>
+      <c r="V90" s="8"/>
+      <c r="W90" s="5"/>
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="11"/>
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
@@ -9245,10 +9359,11 @@
       <c r="R91" s="13"/>
       <c r="S91" s="13"/>
       <c r="T91" s="13"/>
-      <c r="U91" s="8"/>
-      <c r="V91" s="5"/>
-    </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U91" s="23"/>
+      <c r="V91" s="8"/>
+      <c r="W91" s="5"/>
+    </row>
+    <row r="92" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="11"/>
       <c r="B92" s="13"/>
       <c r="C92" s="13"/>
@@ -9269,10 +9384,11 @@
       <c r="R92" s="13"/>
       <c r="S92" s="13"/>
       <c r="T92" s="13"/>
-      <c r="U92" s="8"/>
-      <c r="V92" s="5"/>
-    </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U92" s="23"/>
+      <c r="V92" s="8"/>
+      <c r="W92" s="5"/>
+    </row>
+    <row r="93" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="11"/>
       <c r="B93" s="13"/>
       <c r="C93" s="13"/>
@@ -9293,10 +9409,11 @@
       <c r="R93" s="13"/>
       <c r="S93" s="13"/>
       <c r="T93" s="13"/>
-      <c r="U93" s="8"/>
-      <c r="V93" s="5"/>
-    </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U93" s="23"/>
+      <c r="V93" s="8"/>
+      <c r="W93" s="5"/>
+    </row>
+    <row r="94" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="11"/>
       <c r="B94" s="13"/>
       <c r="C94" s="13"/>
@@ -9317,10 +9434,11 @@
       <c r="R94" s="13"/>
       <c r="S94" s="13"/>
       <c r="T94" s="13"/>
-      <c r="U94" s="8"/>
-      <c r="V94" s="5"/>
-    </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U94" s="23"/>
+      <c r="V94" s="8"/>
+      <c r="W94" s="5"/>
+    </row>
+    <row r="95" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="11"/>
       <c r="B95" s="13"/>
       <c r="C95" s="13"/>
@@ -9341,10 +9459,11 @@
       <c r="R95" s="13"/>
       <c r="S95" s="13"/>
       <c r="T95" s="13"/>
-      <c r="U95" s="8"/>
-      <c r="V95" s="5"/>
-    </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U95" s="23"/>
+      <c r="V95" s="8"/>
+      <c r="W95" s="5"/>
+    </row>
+    <row r="96" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="11"/>
       <c r="B96" s="13"/>
       <c r="C96" s="13"/>
@@ -9365,10 +9484,11 @@
       <c r="R96" s="13"/>
       <c r="S96" s="13"/>
       <c r="T96" s="13"/>
-      <c r="U96" s="8"/>
-      <c r="V96" s="5"/>
-    </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U96" s="23"/>
+      <c r="V96" s="8"/>
+      <c r="W96" s="5"/>
+    </row>
+    <row r="97" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="11"/>
       <c r="B97" s="13"/>
       <c r="C97" s="13"/>
@@ -9389,10 +9509,11 @@
       <c r="R97" s="13"/>
       <c r="S97" s="13"/>
       <c r="T97" s="13"/>
-      <c r="U97" s="8"/>
-      <c r="V97" s="5"/>
-    </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U97" s="23"/>
+      <c r="V97" s="8"/>
+      <c r="W97" s="5"/>
+    </row>
+    <row r="98" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="11"/>
       <c r="B98" s="13"/>
       <c r="C98" s="13"/>
@@ -9413,10 +9534,11 @@
       <c r="R98" s="13"/>
       <c r="S98" s="13"/>
       <c r="T98" s="13"/>
-      <c r="U98" s="8"/>
-      <c r="V98" s="5"/>
-    </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U98" s="23"/>
+      <c r="V98" s="8"/>
+      <c r="W98" s="5"/>
+    </row>
+    <row r="99" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="11"/>
       <c r="B99" s="13"/>
       <c r="C99" s="13"/>
@@ -9437,10 +9559,11 @@
       <c r="R99" s="13"/>
       <c r="S99" s="13"/>
       <c r="T99" s="13"/>
-      <c r="U99" s="8"/>
-      <c r="V99" s="5"/>
-    </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U99" s="23"/>
+      <c r="V99" s="8"/>
+      <c r="W99" s="5"/>
+    </row>
+    <row r="100" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="11"/>
       <c r="B100" s="13"/>
       <c r="C100" s="13"/>
@@ -9461,10 +9584,11 @@
       <c r="R100" s="13"/>
       <c r="S100" s="13"/>
       <c r="T100" s="13"/>
-      <c r="U100" s="8"/>
-      <c r="V100" s="5"/>
-    </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U100" s="23"/>
+      <c r="V100" s="8"/>
+      <c r="W100" s="5"/>
+    </row>
+    <row r="101" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="11"/>
       <c r="B101" s="13"/>
       <c r="C101" s="13"/>
@@ -9485,10 +9609,11 @@
       <c r="R101" s="13"/>
       <c r="S101" s="13"/>
       <c r="T101" s="13"/>
-      <c r="U101" s="8"/>
-      <c r="V101" s="5"/>
-    </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U101" s="23"/>
+      <c r="V101" s="8"/>
+      <c r="W101" s="5"/>
+    </row>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="11"/>
       <c r="B102" s="13"/>
       <c r="C102" s="13"/>
@@ -9509,10 +9634,11 @@
       <c r="R102" s="13"/>
       <c r="S102" s="13"/>
       <c r="T102" s="13"/>
-      <c r="U102" s="8"/>
-      <c r="V102" s="5"/>
-    </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U102" s="23"/>
+      <c r="V102" s="8"/>
+      <c r="W102" s="5"/>
+    </row>
+    <row r="103" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="11"/>
       <c r="B103" s="13"/>
       <c r="C103" s="13"/>
@@ -9533,10 +9659,11 @@
       <c r="R103" s="13"/>
       <c r="S103" s="13"/>
       <c r="T103" s="13"/>
-      <c r="U103" s="8"/>
-      <c r="V103" s="5"/>
-    </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U103" s="23"/>
+      <c r="V103" s="8"/>
+      <c r="W103" s="5"/>
+    </row>
+    <row r="104" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="11"/>
       <c r="B104" s="13"/>
       <c r="C104" s="13"/>
@@ -9557,10 +9684,11 @@
       <c r="R104" s="13"/>
       <c r="S104" s="13"/>
       <c r="T104" s="13"/>
-      <c r="U104" s="8"/>
-      <c r="V104" s="5"/>
-    </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U104" s="23"/>
+      <c r="V104" s="8"/>
+      <c r="W104" s="5"/>
+    </row>
+    <row r="105" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="11"/>
       <c r="B105" s="13"/>
       <c r="C105" s="13"/>
@@ -9581,10 +9709,11 @@
       <c r="R105" s="13"/>
       <c r="S105" s="13"/>
       <c r="T105" s="13"/>
-      <c r="U105" s="8"/>
-      <c r="V105" s="5"/>
-    </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U105" s="23"/>
+      <c r="V105" s="8"/>
+      <c r="W105" s="5"/>
+    </row>
+    <row r="106" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="11"/>
       <c r="B106" s="13"/>
       <c r="C106" s="13"/>
@@ -9605,10 +9734,11 @@
       <c r="R106" s="13"/>
       <c r="S106" s="13"/>
       <c r="T106" s="13"/>
-      <c r="U106" s="8"/>
-      <c r="V106" s="5"/>
-    </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U106" s="23"/>
+      <c r="V106" s="8"/>
+      <c r="W106" s="5"/>
+    </row>
+    <row r="107" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="11"/>
       <c r="B107" s="13"/>
       <c r="C107" s="13"/>
@@ -9629,10 +9759,11 @@
       <c r="R107" s="13"/>
       <c r="S107" s="13"/>
       <c r="T107" s="13"/>
-      <c r="U107" s="8"/>
-      <c r="V107" s="5"/>
-    </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U107" s="23"/>
+      <c r="V107" s="8"/>
+      <c r="W107" s="5"/>
+    </row>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="11"/>
       <c r="B108" s="13"/>
       <c r="C108" s="13"/>
@@ -9653,10 +9784,11 @@
       <c r="R108" s="13"/>
       <c r="S108" s="13"/>
       <c r="T108" s="13"/>
-      <c r="U108" s="8"/>
-      <c r="V108" s="5"/>
-    </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U108" s="23"/>
+      <c r="V108" s="8"/>
+      <c r="W108" s="5"/>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="11"/>
       <c r="B109" s="13"/>
       <c r="C109" s="13"/>
@@ -9677,10 +9809,11 @@
       <c r="R109" s="13"/>
       <c r="S109" s="13"/>
       <c r="T109" s="13"/>
-      <c r="U109" s="8"/>
-      <c r="V109" s="5"/>
-    </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U109" s="23"/>
+      <c r="V109" s="8"/>
+      <c r="W109" s="5"/>
+    </row>
+    <row r="110" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="11"/>
       <c r="B110" s="13"/>
       <c r="C110" s="13"/>
@@ -9701,10 +9834,11 @@
       <c r="R110" s="13"/>
       <c r="S110" s="13"/>
       <c r="T110" s="13"/>
-      <c r="U110" s="8"/>
-      <c r="V110" s="5"/>
-    </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U110" s="23"/>
+      <c r="V110" s="8"/>
+      <c r="W110" s="5"/>
+    </row>
+    <row r="111" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="11"/>
       <c r="B111" s="13"/>
       <c r="C111" s="13"/>
@@ -9725,10 +9859,11 @@
       <c r="R111" s="13"/>
       <c r="S111" s="13"/>
       <c r="T111" s="13"/>
-      <c r="U111" s="8"/>
-      <c r="V111" s="5"/>
-    </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U111" s="23"/>
+      <c r="V111" s="8"/>
+      <c r="W111" s="5"/>
+    </row>
+    <row r="112" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="11"/>
       <c r="B112" s="13"/>
       <c r="C112" s="13"/>
@@ -9749,10 +9884,11 @@
       <c r="R112" s="13"/>
       <c r="S112" s="13"/>
       <c r="T112" s="13"/>
-      <c r="U112" s="8"/>
-      <c r="V112" s="5"/>
-    </row>
-    <row r="113" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U112" s="23"/>
+      <c r="V112" s="8"/>
+      <c r="W112" s="5"/>
+    </row>
+    <row r="113" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="11"/>
       <c r="B113" s="13"/>
       <c r="C113" s="13"/>
@@ -9773,10 +9909,11 @@
       <c r="R113" s="13"/>
       <c r="S113" s="13"/>
       <c r="T113" s="13"/>
-      <c r="U113" s="8"/>
-      <c r="V113" s="5"/>
-    </row>
-    <row r="114" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U113" s="23"/>
+      <c r="V113" s="8"/>
+      <c r="W113" s="5"/>
+    </row>
+    <row r="114" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="11"/>
       <c r="B114" s="13"/>
       <c r="C114" s="13"/>
@@ -9797,10 +9934,11 @@
       <c r="R114" s="13"/>
       <c r="S114" s="13"/>
       <c r="T114" s="13"/>
-      <c r="U114" s="8"/>
-      <c r="V114" s="5"/>
-    </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U114" s="23"/>
+      <c r="V114" s="8"/>
+      <c r="W114" s="5"/>
+    </row>
+    <row r="115" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="11"/>
       <c r="B115" s="13"/>
       <c r="C115" s="13"/>
@@ -9821,10 +9959,11 @@
       <c r="R115" s="13"/>
       <c r="S115" s="13"/>
       <c r="T115" s="13"/>
-      <c r="U115" s="8"/>
-      <c r="V115" s="5"/>
-    </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U115" s="23"/>
+      <c r="V115" s="8"/>
+      <c r="W115" s="5"/>
+    </row>
+    <row r="116" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="11"/>
       <c r="B116" s="13"/>
       <c r="C116" s="13"/>
@@ -9845,10 +9984,11 @@
       <c r="R116" s="13"/>
       <c r="S116" s="13"/>
       <c r="T116" s="13"/>
-      <c r="U116" s="8"/>
-      <c r="V116" s="5"/>
-    </row>
-    <row r="117" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U116" s="23"/>
+      <c r="V116" s="8"/>
+      <c r="W116" s="5"/>
+    </row>
+    <row r="117" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="11"/>
       <c r="B117" s="13"/>
       <c r="C117" s="13"/>
@@ -9869,10 +10009,11 @@
       <c r="R117" s="13"/>
       <c r="S117" s="13"/>
       <c r="T117" s="13"/>
-      <c r="U117" s="8"/>
-      <c r="V117" s="5"/>
-    </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U117" s="23"/>
+      <c r="V117" s="8"/>
+      <c r="W117" s="5"/>
+    </row>
+    <row r="118" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="11"/>
       <c r="B118" s="13"/>
       <c r="C118" s="13"/>
@@ -9893,10 +10034,11 @@
       <c r="R118" s="13"/>
       <c r="S118" s="13"/>
       <c r="T118" s="13"/>
-      <c r="U118" s="8"/>
-      <c r="V118" s="5"/>
-    </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U118" s="23"/>
+      <c r="V118" s="8"/>
+      <c r="W118" s="5"/>
+    </row>
+    <row r="119" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="11"/>
       <c r="B119" s="13"/>
       <c r="C119" s="13"/>
@@ -9917,10 +10059,11 @@
       <c r="R119" s="13"/>
       <c r="S119" s="13"/>
       <c r="T119" s="13"/>
-      <c r="U119" s="8"/>
-      <c r="V119" s="5"/>
-    </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U119" s="23"/>
+      <c r="V119" s="8"/>
+      <c r="W119" s="5"/>
+    </row>
+    <row r="120" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="11"/>
       <c r="B120" s="13"/>
       <c r="C120" s="13"/>
@@ -9941,10 +10084,11 @@
       <c r="R120" s="13"/>
       <c r="S120" s="13"/>
       <c r="T120" s="13"/>
-      <c r="U120" s="8"/>
-      <c r="V120" s="5"/>
-    </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U120" s="23"/>
+      <c r="V120" s="8"/>
+      <c r="W120" s="5"/>
+    </row>
+    <row r="121" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="11"/>
       <c r="B121" s="13"/>
       <c r="C121" s="13"/>
@@ -9965,10 +10109,11 @@
       <c r="R121" s="13"/>
       <c r="S121" s="13"/>
       <c r="T121" s="13"/>
-      <c r="U121" s="8"/>
-      <c r="V121" s="5"/>
-    </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U121" s="23"/>
+      <c r="V121" s="8"/>
+      <c r="W121" s="5"/>
+    </row>
+    <row r="122" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="11"/>
       <c r="B122" s="13"/>
       <c r="C122" s="13"/>
@@ -9989,10 +10134,11 @@
       <c r="R122" s="13"/>
       <c r="S122" s="13"/>
       <c r="T122" s="13"/>
-      <c r="U122" s="8"/>
-      <c r="V122" s="5"/>
-    </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U122" s="23"/>
+      <c r="V122" s="8"/>
+      <c r="W122" s="5"/>
+    </row>
+    <row r="123" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="11"/>
       <c r="B123" s="13"/>
       <c r="C123" s="13"/>
@@ -10013,10 +10159,11 @@
       <c r="R123" s="13"/>
       <c r="S123" s="13"/>
       <c r="T123" s="13"/>
-      <c r="U123" s="8"/>
-      <c r="V123" s="5"/>
-    </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U123" s="23"/>
+      <c r="V123" s="8"/>
+      <c r="W123" s="5"/>
+    </row>
+    <row r="124" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="11"/>
       <c r="B124" s="13"/>
       <c r="C124" s="13"/>
@@ -10037,10 +10184,11 @@
       <c r="R124" s="13"/>
       <c r="S124" s="13"/>
       <c r="T124" s="13"/>
-      <c r="U124" s="8"/>
-      <c r="V124" s="5"/>
-    </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U124" s="23"/>
+      <c r="V124" s="8"/>
+      <c r="W124" s="5"/>
+    </row>
+    <row r="125" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="11"/>
       <c r="B125" s="13"/>
       <c r="C125" s="13"/>
@@ -10061,10 +10209,11 @@
       <c r="R125" s="13"/>
       <c r="S125" s="13"/>
       <c r="T125" s="13"/>
-      <c r="U125" s="8"/>
-      <c r="V125" s="5"/>
-    </row>
-    <row r="126" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U125" s="23"/>
+      <c r="V125" s="8"/>
+      <c r="W125" s="5"/>
+    </row>
+    <row r="126" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="11"/>
       <c r="B126" s="13"/>
       <c r="C126" s="13"/>
@@ -10085,10 +10234,11 @@
       <c r="R126" s="13"/>
       <c r="S126" s="13"/>
       <c r="T126" s="13"/>
-      <c r="U126" s="8"/>
-      <c r="V126" s="5"/>
-    </row>
-    <row r="127" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U126" s="23"/>
+      <c r="V126" s="8"/>
+      <c r="W126" s="5"/>
+    </row>
+    <row r="127" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="11"/>
       <c r="B127" s="13"/>
       <c r="C127" s="13"/>
@@ -10109,10 +10259,11 @@
       <c r="R127" s="13"/>
       <c r="S127" s="13"/>
       <c r="T127" s="13"/>
-      <c r="U127" s="8"/>
-      <c r="V127" s="5"/>
-    </row>
-    <row r="128" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U127" s="23"/>
+      <c r="V127" s="8"/>
+      <c r="W127" s="5"/>
+    </row>
+    <row r="128" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="11"/>
       <c r="B128" s="13"/>
       <c r="C128" s="13"/>
@@ -10133,10 +10284,11 @@
       <c r="R128" s="13"/>
       <c r="S128" s="13"/>
       <c r="T128" s="13"/>
-      <c r="U128" s="8"/>
-      <c r="V128" s="5"/>
-    </row>
-    <row r="129" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U128" s="23"/>
+      <c r="V128" s="8"/>
+      <c r="W128" s="5"/>
+    </row>
+    <row r="129" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="11"/>
       <c r="B129" s="13"/>
       <c r="C129" s="13"/>
@@ -10157,10 +10309,11 @@
       <c r="R129" s="13"/>
       <c r="S129" s="13"/>
       <c r="T129" s="13"/>
-      <c r="U129" s="8"/>
-      <c r="V129" s="5"/>
-    </row>
-    <row r="130" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U129" s="23"/>
+      <c r="V129" s="8"/>
+      <c r="W129" s="5"/>
+    </row>
+    <row r="130" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="11"/>
       <c r="B130" s="13"/>
       <c r="C130" s="13"/>
@@ -10181,10 +10334,11 @@
       <c r="R130" s="13"/>
       <c r="S130" s="13"/>
       <c r="T130" s="13"/>
-      <c r="U130" s="8"/>
-      <c r="V130" s="5"/>
-    </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U130" s="23"/>
+      <c r="V130" s="8"/>
+      <c r="W130" s="5"/>
+    </row>
+    <row r="131" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="11"/>
       <c r="B131" s="13"/>
       <c r="C131" s="13"/>
@@ -10205,10 +10359,11 @@
       <c r="R131" s="13"/>
       <c r="S131" s="13"/>
       <c r="T131" s="13"/>
-      <c r="U131" s="8"/>
-      <c r="V131" s="5"/>
-    </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U131" s="23"/>
+      <c r="V131" s="8"/>
+      <c r="W131" s="5"/>
+    </row>
+    <row r="132" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="11"/>
       <c r="B132" s="13"/>
       <c r="C132" s="13"/>
@@ -10229,10 +10384,11 @@
       <c r="R132" s="13"/>
       <c r="S132" s="13"/>
       <c r="T132" s="13"/>
-      <c r="U132" s="8"/>
-      <c r="V132" s="5"/>
-    </row>
-    <row r="133" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U132" s="23"/>
+      <c r="V132" s="8"/>
+      <c r="W132" s="5"/>
+    </row>
+    <row r="133" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="11"/>
       <c r="B133" s="13"/>
       <c r="C133" s="13"/>
@@ -10253,10 +10409,11 @@
       <c r="R133" s="13"/>
       <c r="S133" s="13"/>
       <c r="T133" s="13"/>
-      <c r="U133" s="8"/>
-      <c r="V133" s="5"/>
-    </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U133" s="23"/>
+      <c r="V133" s="8"/>
+      <c r="W133" s="5"/>
+    </row>
+    <row r="134" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="11"/>
       <c r="B134" s="13"/>
       <c r="C134" s="13"/>
@@ -10277,10 +10434,11 @@
       <c r="R134" s="13"/>
       <c r="S134" s="13"/>
       <c r="T134" s="13"/>
-      <c r="U134" s="8"/>
-      <c r="V134" s="5"/>
-    </row>
-    <row r="135" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U134" s="23"/>
+      <c r="V134" s="8"/>
+      <c r="W134" s="5"/>
+    </row>
+    <row r="135" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="11"/>
       <c r="B135" s="13"/>
       <c r="C135" s="13"/>
@@ -10301,10 +10459,11 @@
       <c r="R135" s="13"/>
       <c r="S135" s="13"/>
       <c r="T135" s="13"/>
-      <c r="U135" s="8"/>
-      <c r="V135" s="5"/>
-    </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U135" s="23"/>
+      <c r="V135" s="8"/>
+      <c r="W135" s="5"/>
+    </row>
+    <row r="136" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="11"/>
       <c r="B136" s="13"/>
       <c r="C136" s="13"/>
@@ -10325,10 +10484,11 @@
       <c r="R136" s="13"/>
       <c r="S136" s="13"/>
       <c r="T136" s="13"/>
-      <c r="U136" s="8"/>
-      <c r="V136" s="5"/>
-    </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U136" s="23"/>
+      <c r="V136" s="8"/>
+      <c r="W136" s="5"/>
+    </row>
+    <row r="137" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="11"/>
       <c r="B137" s="13"/>
       <c r="C137" s="13"/>
@@ -10349,10 +10509,11 @@
       <c r="R137" s="13"/>
       <c r="S137" s="13"/>
       <c r="T137" s="13"/>
-      <c r="U137" s="8"/>
-      <c r="V137" s="5"/>
-    </row>
-    <row r="138" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U137" s="23"/>
+      <c r="V137" s="8"/>
+      <c r="W137" s="5"/>
+    </row>
+    <row r="138" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="11"/>
       <c r="B138" s="13"/>
       <c r="C138" s="13"/>
@@ -10373,10 +10534,11 @@
       <c r="R138" s="13"/>
       <c r="S138" s="13"/>
       <c r="T138" s="13"/>
-      <c r="U138" s="8"/>
-      <c r="V138" s="5"/>
-    </row>
-    <row r="139" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U138" s="23"/>
+      <c r="V138" s="8"/>
+      <c r="W138" s="5"/>
+    </row>
+    <row r="139" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="11"/>
       <c r="B139" s="13"/>
       <c r="C139" s="13"/>
@@ -10397,10 +10559,11 @@
       <c r="R139" s="13"/>
       <c r="S139" s="13"/>
       <c r="T139" s="13"/>
-      <c r="U139" s="8"/>
-      <c r="V139" s="5"/>
-    </row>
-    <row r="140" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U139" s="23"/>
+      <c r="V139" s="8"/>
+      <c r="W139" s="5"/>
+    </row>
+    <row r="140" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="11"/>
       <c r="B140" s="13"/>
       <c r="C140" s="13"/>
@@ -10421,10 +10584,11 @@
       <c r="R140" s="13"/>
       <c r="S140" s="13"/>
       <c r="T140" s="13"/>
-      <c r="U140" s="8"/>
-      <c r="V140" s="5"/>
-    </row>
-    <row r="141" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U140" s="23"/>
+      <c r="V140" s="8"/>
+      <c r="W140" s="5"/>
+    </row>
+    <row r="141" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="11"/>
       <c r="B141" s="13"/>
       <c r="C141" s="13"/>
@@ -10445,10 +10609,11 @@
       <c r="R141" s="13"/>
       <c r="S141" s="13"/>
       <c r="T141" s="13"/>
-      <c r="U141" s="8"/>
-      <c r="V141" s="5"/>
-    </row>
-    <row r="142" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U141" s="23"/>
+      <c r="V141" s="8"/>
+      <c r="W141" s="5"/>
+    </row>
+    <row r="142" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="11"/>
       <c r="B142" s="13"/>
       <c r="C142" s="13"/>
@@ -10469,10 +10634,11 @@
       <c r="R142" s="13"/>
       <c r="S142" s="13"/>
       <c r="T142" s="13"/>
-      <c r="U142" s="8"/>
-      <c r="V142" s="5"/>
-    </row>
-    <row r="143" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U142" s="23"/>
+      <c r="V142" s="8"/>
+      <c r="W142" s="5"/>
+    </row>
+    <row r="143" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="11"/>
       <c r="B143" s="13"/>
       <c r="C143" s="13"/>
@@ -10493,10 +10659,11 @@
       <c r="R143" s="13"/>
       <c r="S143" s="13"/>
       <c r="T143" s="13"/>
-      <c r="U143" s="8"/>
-      <c r="V143" s="5"/>
-    </row>
-    <row r="144" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U143" s="23"/>
+      <c r="V143" s="8"/>
+      <c r="W143" s="5"/>
+    </row>
+    <row r="144" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="11"/>
       <c r="B144" s="13"/>
       <c r="C144" s="13"/>
@@ -10517,10 +10684,11 @@
       <c r="R144" s="13"/>
       <c r="S144" s="13"/>
       <c r="T144" s="13"/>
-      <c r="U144" s="8"/>
-      <c r="V144" s="5"/>
-    </row>
-    <row r="145" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U144" s="23"/>
+      <c r="V144" s="8"/>
+      <c r="W144" s="5"/>
+    </row>
+    <row r="145" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="11"/>
       <c r="B145" s="13"/>
       <c r="C145" s="13"/>
@@ -10541,10 +10709,11 @@
       <c r="R145" s="13"/>
       <c r="S145" s="13"/>
       <c r="T145" s="13"/>
-      <c r="U145" s="8"/>
-      <c r="V145" s="5"/>
-    </row>
-    <row r="146" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U145" s="23"/>
+      <c r="V145" s="8"/>
+      <c r="W145" s="5"/>
+    </row>
+    <row r="146" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="11"/>
       <c r="B146" s="13"/>
       <c r="C146" s="13"/>
@@ -10565,10 +10734,11 @@
       <c r="R146" s="13"/>
       <c r="S146" s="13"/>
       <c r="T146" s="13"/>
-      <c r="U146" s="8"/>
-      <c r="V146" s="5"/>
-    </row>
-    <row r="147" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U146" s="23"/>
+      <c r="V146" s="8"/>
+      <c r="W146" s="5"/>
+    </row>
+    <row r="147" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="11"/>
       <c r="B147" s="13"/>
       <c r="C147" s="13"/>
@@ -10589,10 +10759,11 @@
       <c r="R147" s="13"/>
       <c r="S147" s="13"/>
       <c r="T147" s="13"/>
-      <c r="U147" s="8"/>
-      <c r="V147" s="5"/>
-    </row>
-    <row r="148" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U147" s="23"/>
+      <c r="V147" s="8"/>
+      <c r="W147" s="5"/>
+    </row>
+    <row r="148" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="11"/>
       <c r="B148" s="13"/>
       <c r="C148" s="13"/>
@@ -10613,10 +10784,11 @@
       <c r="R148" s="13"/>
       <c r="S148" s="13"/>
       <c r="T148" s="13"/>
-      <c r="U148" s="8"/>
-      <c r="V148" s="5"/>
-    </row>
-    <row r="149" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U148" s="23"/>
+      <c r="V148" s="8"/>
+      <c r="W148" s="5"/>
+    </row>
+    <row r="149" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="11"/>
       <c r="B149" s="13"/>
       <c r="C149" s="13"/>
@@ -10637,10 +10809,11 @@
       <c r="R149" s="13"/>
       <c r="S149" s="13"/>
       <c r="T149" s="13"/>
-      <c r="U149" s="8"/>
-      <c r="V149" s="5"/>
-    </row>
-    <row r="150" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U149" s="23"/>
+      <c r="V149" s="8"/>
+      <c r="W149" s="5"/>
+    </row>
+    <row r="150" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="11"/>
       <c r="B150" s="13"/>
       <c r="C150" s="13"/>
@@ -10661,10 +10834,11 @@
       <c r="R150" s="13"/>
       <c r="S150" s="13"/>
       <c r="T150" s="13"/>
-      <c r="U150" s="8"/>
-      <c r="V150" s="5"/>
-    </row>
-    <row r="151" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U150" s="23"/>
+      <c r="V150" s="8"/>
+      <c r="W150" s="5"/>
+    </row>
+    <row r="151" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="11"/>
       <c r="B151" s="13"/>
       <c r="C151" s="13"/>
@@ -10685,10 +10859,11 @@
       <c r="R151" s="13"/>
       <c r="S151" s="13"/>
       <c r="T151" s="13"/>
-      <c r="U151" s="8"/>
-      <c r="V151" s="5"/>
-    </row>
-    <row r="152" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U151" s="23"/>
+      <c r="V151" s="8"/>
+      <c r="W151" s="5"/>
+    </row>
+    <row r="152" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="11"/>
       <c r="B152" s="13"/>
       <c r="C152" s="13"/>
@@ -10709,10 +10884,11 @@
       <c r="R152" s="13"/>
       <c r="S152" s="13"/>
       <c r="T152" s="13"/>
-      <c r="U152" s="8"/>
-      <c r="V152" s="5"/>
-    </row>
-    <row r="153" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U152" s="23"/>
+      <c r="V152" s="8"/>
+      <c r="W152" s="5"/>
+    </row>
+    <row r="153" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="11"/>
       <c r="B153" s="13"/>
       <c r="C153" s="13"/>
@@ -10733,10 +10909,11 @@
       <c r="R153" s="13"/>
       <c r="S153" s="13"/>
       <c r="T153" s="13"/>
-      <c r="U153" s="8"/>
-      <c r="V153" s="5"/>
-    </row>
-    <row r="154" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U153" s="23"/>
+      <c r="V153" s="8"/>
+      <c r="W153" s="5"/>
+    </row>
+    <row r="154" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="11"/>
       <c r="B154" s="13"/>
       <c r="C154" s="13"/>
@@ -10757,10 +10934,11 @@
       <c r="R154" s="13"/>
       <c r="S154" s="13"/>
       <c r="T154" s="13"/>
-      <c r="U154" s="8"/>
-      <c r="V154" s="5"/>
-    </row>
-    <row r="155" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U154" s="23"/>
+      <c r="V154" s="8"/>
+      <c r="W154" s="5"/>
+    </row>
+    <row r="155" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="11"/>
       <c r="B155" s="13"/>
       <c r="C155" s="13"/>
@@ -10781,10 +10959,11 @@
       <c r="R155" s="13"/>
       <c r="S155" s="13"/>
       <c r="T155" s="13"/>
-      <c r="U155" s="8"/>
-      <c r="V155" s="5"/>
-    </row>
-    <row r="156" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U155" s="23"/>
+      <c r="V155" s="8"/>
+      <c r="W155" s="5"/>
+    </row>
+    <row r="156" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="11"/>
       <c r="B156" s="13"/>
       <c r="C156" s="13"/>
@@ -10805,10 +10984,11 @@
       <c r="R156" s="13"/>
       <c r="S156" s="13"/>
       <c r="T156" s="13"/>
-      <c r="U156" s="8"/>
-      <c r="V156" s="5"/>
-    </row>
-    <row r="157" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U156" s="23"/>
+      <c r="V156" s="8"/>
+      <c r="W156" s="5"/>
+    </row>
+    <row r="157" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="11"/>
       <c r="B157" s="13"/>
       <c r="C157" s="13"/>
@@ -10829,10 +11009,11 @@
       <c r="R157" s="13"/>
       <c r="S157" s="13"/>
       <c r="T157" s="13"/>
-      <c r="U157" s="8"/>
-      <c r="V157" s="5"/>
-    </row>
-    <row r="158" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U157" s="23"/>
+      <c r="V157" s="8"/>
+      <c r="W157" s="5"/>
+    </row>
+    <row r="158" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="11"/>
       <c r="B158" s="13"/>
       <c r="C158" s="13"/>
@@ -10853,10 +11034,11 @@
       <c r="R158" s="13"/>
       <c r="S158" s="13"/>
       <c r="T158" s="13"/>
-      <c r="U158" s="8"/>
-      <c r="V158" s="5"/>
-    </row>
-    <row r="159" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U158" s="23"/>
+      <c r="V158" s="8"/>
+      <c r="W158" s="5"/>
+    </row>
+    <row r="159" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="11"/>
       <c r="B159" s="13"/>
       <c r="C159" s="13"/>
@@ -10877,10 +11059,11 @@
       <c r="R159" s="13"/>
       <c r="S159" s="13"/>
       <c r="T159" s="13"/>
-      <c r="U159" s="8"/>
-      <c r="V159" s="5"/>
-    </row>
-    <row r="160" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U159" s="23"/>
+      <c r="V159" s="8"/>
+      <c r="W159" s="5"/>
+    </row>
+    <row r="160" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="11"/>
       <c r="B160" s="13"/>
       <c r="C160" s="13"/>
@@ -10901,10 +11084,11 @@
       <c r="R160" s="13"/>
       <c r="S160" s="13"/>
       <c r="T160" s="13"/>
-      <c r="U160" s="8"/>
-      <c r="V160" s="5"/>
-    </row>
-    <row r="161" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U160" s="23"/>
+      <c r="V160" s="8"/>
+      <c r="W160" s="5"/>
+    </row>
+    <row r="161" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="11"/>
       <c r="B161" s="13"/>
       <c r="C161" s="13"/>
@@ -10925,10 +11109,11 @@
       <c r="R161" s="13"/>
       <c r="S161" s="13"/>
       <c r="T161" s="13"/>
-      <c r="U161" s="8"/>
-      <c r="V161" s="5"/>
-    </row>
-    <row r="162" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U161" s="23"/>
+      <c r="V161" s="8"/>
+      <c r="W161" s="5"/>
+    </row>
+    <row r="162" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="11"/>
       <c r="B162" s="13"/>
       <c r="C162" s="13"/>
@@ -10949,10 +11134,11 @@
       <c r="R162" s="13"/>
       <c r="S162" s="13"/>
       <c r="T162" s="13"/>
-      <c r="U162" s="8"/>
-      <c r="V162" s="5"/>
-    </row>
-    <row r="163" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U162" s="23"/>
+      <c r="V162" s="8"/>
+      <c r="W162" s="5"/>
+    </row>
+    <row r="163" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="11"/>
       <c r="B163" s="13"/>
       <c r="C163" s="13"/>
@@ -10973,10 +11159,11 @@
       <c r="R163" s="13"/>
       <c r="S163" s="13"/>
       <c r="T163" s="13"/>
-      <c r="U163" s="8"/>
-      <c r="V163" s="5"/>
-    </row>
-    <row r="164" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U163" s="23"/>
+      <c r="V163" s="8"/>
+      <c r="W163" s="5"/>
+    </row>
+    <row r="164" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="11"/>
       <c r="B164" s="13"/>
       <c r="C164" s="13"/>
@@ -10997,10 +11184,11 @@
       <c r="R164" s="13"/>
       <c r="S164" s="13"/>
       <c r="T164" s="13"/>
-      <c r="U164" s="8"/>
-      <c r="V164" s="5"/>
-    </row>
-    <row r="165" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U164" s="23"/>
+      <c r="V164" s="8"/>
+      <c r="W164" s="5"/>
+    </row>
+    <row r="165" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="11"/>
       <c r="B165" s="13"/>
       <c r="C165" s="13"/>
@@ -11021,10 +11209,11 @@
       <c r="R165" s="13"/>
       <c r="S165" s="13"/>
       <c r="T165" s="13"/>
-      <c r="U165" s="8"/>
-      <c r="V165" s="5"/>
-    </row>
-    <row r="166" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U165" s="23"/>
+      <c r="V165" s="8"/>
+      <c r="W165" s="5"/>
+    </row>
+    <row r="166" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="11"/>
       <c r="B166" s="13"/>
       <c r="C166" s="13"/>
@@ -11045,10 +11234,11 @@
       <c r="R166" s="13"/>
       <c r="S166" s="13"/>
       <c r="T166" s="13"/>
-      <c r="U166" s="8"/>
-      <c r="V166" s="5"/>
-    </row>
-    <row r="167" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U166" s="23"/>
+      <c r="V166" s="8"/>
+      <c r="W166" s="5"/>
+    </row>
+    <row r="167" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="11"/>
       <c r="B167" s="13"/>
       <c r="C167" s="13"/>
@@ -11069,10 +11259,11 @@
       <c r="R167" s="13"/>
       <c r="S167" s="13"/>
       <c r="T167" s="13"/>
-      <c r="U167" s="8"/>
-      <c r="V167" s="5"/>
-    </row>
-    <row r="168" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U167" s="23"/>
+      <c r="V167" s="8"/>
+      <c r="W167" s="5"/>
+    </row>
+    <row r="168" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="11"/>
       <c r="B168" s="13"/>
       <c r="C168" s="13"/>
@@ -11093,10 +11284,11 @@
       <c r="R168" s="13"/>
       <c r="S168" s="13"/>
       <c r="T168" s="13"/>
-      <c r="U168" s="8"/>
-      <c r="V168" s="5"/>
-    </row>
-    <row r="169" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U168" s="23"/>
+      <c r="V168" s="8"/>
+      <c r="W168" s="5"/>
+    </row>
+    <row r="169" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="11"/>
       <c r="B169" s="13"/>
       <c r="C169" s="13"/>
@@ -11117,10 +11309,11 @@
       <c r="R169" s="13"/>
       <c r="S169" s="13"/>
       <c r="T169" s="13"/>
-      <c r="U169" s="8"/>
-      <c r="V169" s="5"/>
-    </row>
-    <row r="170" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U169" s="23"/>
+      <c r="V169" s="8"/>
+      <c r="W169" s="5"/>
+    </row>
+    <row r="170" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="11"/>
       <c r="B170" s="13"/>
       <c r="C170" s="13"/>
@@ -11141,10 +11334,11 @@
       <c r="R170" s="13"/>
       <c r="S170" s="13"/>
       <c r="T170" s="13"/>
-      <c r="U170" s="8"/>
-      <c r="V170" s="5"/>
-    </row>
-    <row r="171" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U170" s="23"/>
+      <c r="V170" s="8"/>
+      <c r="W170" s="5"/>
+    </row>
+    <row r="171" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="11"/>
       <c r="B171" s="13"/>
       <c r="C171" s="13"/>
@@ -11165,10 +11359,11 @@
       <c r="R171" s="13"/>
       <c r="S171" s="13"/>
       <c r="T171" s="13"/>
-      <c r="U171" s="8"/>
-      <c r="V171" s="5"/>
-    </row>
-    <row r="172" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U171" s="23"/>
+      <c r="V171" s="8"/>
+      <c r="W171" s="5"/>
+    </row>
+    <row r="172" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="11"/>
       <c r="B172" s="13"/>
       <c r="C172" s="13"/>
@@ -11189,10 +11384,11 @@
       <c r="R172" s="13"/>
       <c r="S172" s="13"/>
       <c r="T172" s="13"/>
-      <c r="U172" s="8"/>
-      <c r="V172" s="5"/>
-    </row>
-    <row r="173" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U172" s="23"/>
+      <c r="V172" s="8"/>
+      <c r="W172" s="5"/>
+    </row>
+    <row r="173" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="11"/>
       <c r="B173" s="13"/>
       <c r="C173" s="13"/>
@@ -11213,10 +11409,11 @@
       <c r="R173" s="13"/>
       <c r="S173" s="13"/>
       <c r="T173" s="13"/>
-      <c r="U173" s="8"/>
-      <c r="V173" s="5"/>
-    </row>
-    <row r="174" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U173" s="23"/>
+      <c r="V173" s="8"/>
+      <c r="W173" s="5"/>
+    </row>
+    <row r="174" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="11"/>
       <c r="B174" s="13"/>
       <c r="C174" s="13"/>
@@ -11237,10 +11434,11 @@
       <c r="R174" s="13"/>
       <c r="S174" s="13"/>
       <c r="T174" s="13"/>
-      <c r="U174" s="8"/>
-      <c r="V174" s="5"/>
-    </row>
-    <row r="175" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U174" s="23"/>
+      <c r="V174" s="8"/>
+      <c r="W174" s="5"/>
+    </row>
+    <row r="175" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="11"/>
       <c r="B175" s="13"/>
       <c r="C175" s="13"/>
@@ -11261,10 +11459,11 @@
       <c r="R175" s="13"/>
       <c r="S175" s="13"/>
       <c r="T175" s="13"/>
-      <c r="U175" s="8"/>
-      <c r="V175" s="5"/>
-    </row>
-    <row r="176" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U175" s="23"/>
+      <c r="V175" s="8"/>
+      <c r="W175" s="5"/>
+    </row>
+    <row r="176" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="11"/>
       <c r="B176" s="13"/>
       <c r="C176" s="13"/>
@@ -11285,10 +11484,11 @@
       <c r="R176" s="13"/>
       <c r="S176" s="13"/>
       <c r="T176" s="13"/>
-      <c r="U176" s="8"/>
-      <c r="V176" s="5"/>
-    </row>
-    <row r="177" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U176" s="23"/>
+      <c r="V176" s="8"/>
+      <c r="W176" s="5"/>
+    </row>
+    <row r="177" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="11"/>
       <c r="B177" s="13"/>
       <c r="C177" s="13"/>
@@ -11309,10 +11509,11 @@
       <c r="R177" s="13"/>
       <c r="S177" s="13"/>
       <c r="T177" s="13"/>
-      <c r="U177" s="8"/>
-      <c r="V177" s="5"/>
-    </row>
-    <row r="178" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U177" s="23"/>
+      <c r="V177" s="8"/>
+      <c r="W177" s="5"/>
+    </row>
+    <row r="178" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="11"/>
       <c r="B178" s="13"/>
       <c r="C178" s="13"/>
@@ -11333,10 +11534,11 @@
       <c r="R178" s="13"/>
       <c r="S178" s="13"/>
       <c r="T178" s="13"/>
-      <c r="U178" s="8"/>
-      <c r="V178" s="5"/>
-    </row>
-    <row r="179" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U178" s="23"/>
+      <c r="V178" s="8"/>
+      <c r="W178" s="5"/>
+    </row>
+    <row r="179" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="11"/>
       <c r="B179" s="13"/>
       <c r="C179" s="13"/>
@@ -11357,10 +11559,11 @@
       <c r="R179" s="13"/>
       <c r="S179" s="13"/>
       <c r="T179" s="13"/>
-      <c r="U179" s="8"/>
-      <c r="V179" s="5"/>
-    </row>
-    <row r="180" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U179" s="23"/>
+      <c r="V179" s="8"/>
+      <c r="W179" s="5"/>
+    </row>
+    <row r="180" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="11"/>
       <c r="B180" s="13"/>
       <c r="C180" s="13"/>
@@ -11381,10 +11584,11 @@
       <c r="R180" s="13"/>
       <c r="S180" s="13"/>
       <c r="T180" s="13"/>
-      <c r="U180" s="8"/>
-      <c r="V180" s="5"/>
-    </row>
-    <row r="181" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U180" s="23"/>
+      <c r="V180" s="8"/>
+      <c r="W180" s="5"/>
+    </row>
+    <row r="181" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="11"/>
       <c r="B181" s="13"/>
       <c r="C181" s="13"/>
@@ -11405,10 +11609,11 @@
       <c r="R181" s="13"/>
       <c r="S181" s="13"/>
       <c r="T181" s="13"/>
-      <c r="U181" s="8"/>
-      <c r="V181" s="5"/>
-    </row>
-    <row r="182" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U181" s="23"/>
+      <c r="V181" s="8"/>
+      <c r="W181" s="5"/>
+    </row>
+    <row r="182" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="11"/>
       <c r="B182" s="13"/>
       <c r="C182" s="13"/>
@@ -11429,10 +11634,11 @@
       <c r="R182" s="13"/>
       <c r="S182" s="13"/>
       <c r="T182" s="13"/>
-      <c r="U182" s="8"/>
-      <c r="V182" s="5"/>
-    </row>
-    <row r="183" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U182" s="23"/>
+      <c r="V182" s="8"/>
+      <c r="W182" s="5"/>
+    </row>
+    <row r="183" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="11"/>
       <c r="B183" s="13"/>
       <c r="C183" s="13"/>
@@ -11453,10 +11659,11 @@
       <c r="R183" s="13"/>
       <c r="S183" s="13"/>
       <c r="T183" s="13"/>
-      <c r="U183" s="8"/>
-      <c r="V183" s="5"/>
-    </row>
-    <row r="184" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U183" s="23"/>
+      <c r="V183" s="8"/>
+      <c r="W183" s="5"/>
+    </row>
+    <row r="184" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="11"/>
       <c r="B184" s="13"/>
       <c r="C184" s="13"/>
@@ -11477,10 +11684,11 @@
       <c r="R184" s="13"/>
       <c r="S184" s="13"/>
       <c r="T184" s="13"/>
-      <c r="U184" s="8"/>
-      <c r="V184" s="5"/>
-    </row>
-    <row r="185" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U184" s="23"/>
+      <c r="V184" s="8"/>
+      <c r="W184" s="5"/>
+    </row>
+    <row r="185" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="11"/>
       <c r="B185" s="13"/>
       <c r="C185" s="13"/>
@@ -11501,10 +11709,11 @@
       <c r="R185" s="13"/>
       <c r="S185" s="13"/>
       <c r="T185" s="13"/>
-      <c r="U185" s="8"/>
-      <c r="V185" s="5"/>
-    </row>
-    <row r="186" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U185" s="23"/>
+      <c r="V185" s="8"/>
+      <c r="W185" s="5"/>
+    </row>
+    <row r="186" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="11"/>
       <c r="B186" s="13"/>
       <c r="C186" s="13"/>
@@ -11525,10 +11734,11 @@
       <c r="R186" s="13"/>
       <c r="S186" s="13"/>
       <c r="T186" s="13"/>
-      <c r="U186" s="8"/>
-      <c r="V186" s="5"/>
-    </row>
-    <row r="187" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U186" s="23"/>
+      <c r="V186" s="8"/>
+      <c r="W186" s="5"/>
+    </row>
+    <row r="187" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="11"/>
       <c r="B187" s="13"/>
       <c r="C187" s="13"/>
@@ -11549,10 +11759,11 @@
       <c r="R187" s="13"/>
       <c r="S187" s="13"/>
       <c r="T187" s="13"/>
-      <c r="U187" s="8"/>
-      <c r="V187" s="5"/>
-    </row>
-    <row r="188" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U187" s="23"/>
+      <c r="V187" s="8"/>
+      <c r="W187" s="5"/>
+    </row>
+    <row r="188" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="11"/>
       <c r="B188" s="13"/>
       <c r="C188" s="13"/>
@@ -11573,10 +11784,11 @@
       <c r="R188" s="13"/>
       <c r="S188" s="13"/>
       <c r="T188" s="13"/>
-      <c r="U188" s="8"/>
-      <c r="V188" s="5"/>
-    </row>
-    <row r="189" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U188" s="23"/>
+      <c r="V188" s="8"/>
+      <c r="W188" s="5"/>
+    </row>
+    <row r="189" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="11"/>
       <c r="B189" s="13"/>
       <c r="C189" s="13"/>
@@ -11597,10 +11809,11 @@
       <c r="R189" s="13"/>
       <c r="S189" s="13"/>
       <c r="T189" s="13"/>
-      <c r="U189" s="8"/>
-      <c r="V189" s="5"/>
-    </row>
-    <row r="190" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U189" s="23"/>
+      <c r="V189" s="8"/>
+      <c r="W189" s="5"/>
+    </row>
+    <row r="190" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="11"/>
       <c r="B190" s="13"/>
       <c r="C190" s="13"/>
@@ -11621,10 +11834,11 @@
       <c r="R190" s="13"/>
       <c r="S190" s="13"/>
       <c r="T190" s="13"/>
-      <c r="U190" s="8"/>
-      <c r="V190" s="5"/>
-    </row>
-    <row r="191" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U190" s="23"/>
+      <c r="V190" s="8"/>
+      <c r="W190" s="5"/>
+    </row>
+    <row r="191" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="11"/>
       <c r="B191" s="13"/>
       <c r="C191" s="13"/>
@@ -11645,10 +11859,11 @@
       <c r="R191" s="13"/>
       <c r="S191" s="13"/>
       <c r="T191" s="13"/>
-      <c r="U191" s="8"/>
-      <c r="V191" s="5"/>
-    </row>
-    <row r="192" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U191" s="23"/>
+      <c r="V191" s="8"/>
+      <c r="W191" s="5"/>
+    </row>
+    <row r="192" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="11"/>
       <c r="B192" s="13"/>
       <c r="C192" s="13"/>
@@ -11669,10 +11884,11 @@
       <c r="R192" s="13"/>
       <c r="S192" s="13"/>
       <c r="T192" s="13"/>
-      <c r="U192" s="8"/>
-      <c r="V192" s="5"/>
-    </row>
-    <row r="193" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U192" s="23"/>
+      <c r="V192" s="8"/>
+      <c r="W192" s="5"/>
+    </row>
+    <row r="193" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="11"/>
       <c r="B193" s="13"/>
       <c r="C193" s="13"/>
@@ -11693,10 +11909,11 @@
       <c r="R193" s="13"/>
       <c r="S193" s="13"/>
       <c r="T193" s="13"/>
-      <c r="U193" s="8"/>
-      <c r="V193" s="5"/>
-    </row>
-    <row r="194" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U193" s="23"/>
+      <c r="V193" s="8"/>
+      <c r="W193" s="5"/>
+    </row>
+    <row r="194" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="11"/>
       <c r="B194" s="13"/>
       <c r="C194" s="13"/>
@@ -11717,10 +11934,11 @@
       <c r="R194" s="13"/>
       <c r="S194" s="13"/>
       <c r="T194" s="13"/>
-      <c r="U194" s="8"/>
-      <c r="V194" s="5"/>
-    </row>
-    <row r="195" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U194" s="23"/>
+      <c r="V194" s="8"/>
+      <c r="W194" s="5"/>
+    </row>
+    <row r="195" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="11"/>
       <c r="B195" s="13"/>
       <c r="C195" s="13"/>
@@ -11741,10 +11959,11 @@
       <c r="R195" s="13"/>
       <c r="S195" s="13"/>
       <c r="T195" s="13"/>
-      <c r="U195" s="8"/>
-      <c r="V195" s="5"/>
-    </row>
-    <row r="196" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U195" s="23"/>
+      <c r="V195" s="8"/>
+      <c r="W195" s="5"/>
+    </row>
+    <row r="196" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="11"/>
       <c r="B196" s="13"/>
       <c r="C196" s="13"/>
@@ -11765,10 +11984,11 @@
       <c r="R196" s="13"/>
       <c r="S196" s="13"/>
       <c r="T196" s="13"/>
-      <c r="U196" s="8"/>
-      <c r="V196" s="5"/>
-    </row>
-    <row r="197" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U196" s="23"/>
+      <c r="V196" s="8"/>
+      <c r="W196" s="5"/>
+    </row>
+    <row r="197" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="11"/>
       <c r="B197" s="13"/>
       <c r="C197" s="13"/>
@@ -11789,10 +12009,11 @@
       <c r="R197" s="13"/>
       <c r="S197" s="13"/>
       <c r="T197" s="13"/>
-      <c r="U197" s="8"/>
-      <c r="V197" s="5"/>
-    </row>
-    <row r="198" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U197" s="23"/>
+      <c r="V197" s="8"/>
+      <c r="W197" s="5"/>
+    </row>
+    <row r="198" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="11"/>
       <c r="B198" s="13"/>
       <c r="C198" s="13"/>
@@ -11813,10 +12034,11 @@
       <c r="R198" s="13"/>
       <c r="S198" s="13"/>
       <c r="T198" s="13"/>
-      <c r="U198" s="8"/>
-      <c r="V198" s="5"/>
-    </row>
-    <row r="199" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U198" s="23"/>
+      <c r="V198" s="8"/>
+      <c r="W198" s="5"/>
+    </row>
+    <row r="199" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="11"/>
       <c r="B199" s="13"/>
       <c r="C199" s="13"/>
@@ -11837,10 +12059,11 @@
       <c r="R199" s="13"/>
       <c r="S199" s="13"/>
       <c r="T199" s="13"/>
-      <c r="U199" s="8"/>
-      <c r="V199" s="5"/>
-    </row>
-    <row r="200" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U199" s="23"/>
+      <c r="V199" s="8"/>
+      <c r="W199" s="5"/>
+    </row>
+    <row r="200" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="11"/>
       <c r="B200" s="13"/>
       <c r="C200" s="13"/>
@@ -11861,10 +12084,11 @@
       <c r="R200" s="13"/>
       <c r="S200" s="13"/>
       <c r="T200" s="13"/>
-      <c r="U200" s="8"/>
-      <c r="V200" s="5"/>
-    </row>
-    <row r="201" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="U200" s="23"/>
+      <c r="V200" s="8"/>
+      <c r="W200" s="5"/>
+    </row>
+    <row r="201" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="12"/>
       <c r="B201" s="14"/>
       <c r="C201" s="14"/>
@@ -11885,13 +12109,14 @@
       <c r="R201" s="14"/>
       <c r="S201" s="14"/>
       <c r="T201" s="14"/>
-      <c r="U201" s="8"/>
-      <c r="V201" s="5"/>
+      <c r="U201" s="23"/>
+      <c r="V201" s="8"/>
+      <c r="W201" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Trigger ID" error="Trigger ID must be an integer greater than 0." sqref="U2:U1048576" xr:uid="{833FFF82-EF89-473C-B621-746362CC677C}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Trigger ID" error="Trigger ID must be an integer greater than 0." sqref="V2:V1048576" xr:uid="{833FFF82-EF89-473C-B621-746362CC677C}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Enabled Option" error="Please select a supported Enabled option." sqref="C2:C1048576" xr:uid="{FD0F90A3-EA67-4EF1-8FA8-3E985A5E4965}">

</xml_diff>

<commit_message>
JP-1485: Get Robot IDs for Get Triggers when target is specific robots
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Triggers.xlsx
+++ b/Workbooks/EN/Triggers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A83034E-CDE1-447A-80C8-C082D0246B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A21964-9FE6-4E2E-9A97-65C71EBA3AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Get" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>Result</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>Use Calendar</t>
-  </si>
-  <si>
-    <t>Start Strategy</t>
   </si>
   <si>
     <t>Start Process Cron</t>
@@ -115,6 +112,14 @@
   <si>
     <t>Start Strategy (Execute XX times)</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start Strategy (-1 All Robots;0 Specific Robots;&gt;0 Execute XX times)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Specified Robot ID's</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -381,7 +386,32 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="56">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -1751,31 +1781,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:V201" headerRowDxfId="54" dataDxfId="52" totalsRowDxfId="50" headerRowBorderDxfId="53" tableBorderDxfId="51">
-  <autoFilter ref="A1:V201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="22">
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Folder ID" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{058B7C0E-F18D-4AA8-A7A4-2A2B65B79498}" name="Folder Name" dataDxfId="48"/>
-    <tableColumn id="1" xr3:uid="{6FFDE20C-2159-4C8B-AE94-46A18EBF32E7}" name="Trigger ID" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{81F71C1A-632D-4A5F-BC94-CC97DF7A65EF}" name="Trigger Name" dataDxfId="46"/>
-    <tableColumn id="17" xr3:uid="{E6C314EE-6A01-4E6A-AF88-E0387E29802E}" name="Enabled" dataDxfId="45"/>
-    <tableColumn id="15" xr3:uid="{2DEE6F64-66B8-46E2-8DED-978C18789A63}" name="Process Name" dataDxfId="44"/>
-    <tableColumn id="14" xr3:uid="{6AFD31D0-7236-4B61-B6F7-B7E209179C91}" name="Input Arguments Definition" dataDxfId="43"/>
-    <tableColumn id="13" xr3:uid="{DB22136F-7CCB-43B3-B2F3-F64F00569B2B}" name="Use Calendar" dataDxfId="42"/>
-    <tableColumn id="12" xr3:uid="{4B4F4CCE-4592-4435-91E9-4E3F0FE0353D}" name="Start Strategy" dataDxfId="41"/>
-    <tableColumn id="11" xr3:uid="{6382E3E3-5FAD-4667-9BD7-D16BEF5953FF}" name="Start Process Cron" dataDxfId="40"/>
-    <tableColumn id="10" xr3:uid="{7A8F0FC9-8380-4F42-9505-29FB8CBCB859}" name="Start Process Cron Details" dataDxfId="39"/>
-    <tableColumn id="9" xr3:uid="{AF0F06BF-7B1B-43E6-A374-D2A97BE7CA57}" name="Stop Strategy" dataDxfId="38"/>
-    <tableColumn id="22" xr3:uid="{E47DF96B-8D93-4081-8137-B872BBA545F0}" name="Stop Process Date" dataDxfId="37"/>
-    <tableColumn id="21" xr3:uid="{5505F1C6-570D-45E3-9390-0F6EFEE4654C}" name="Stop Process Expression" dataDxfId="36"/>
-    <tableColumn id="20" xr3:uid="{5FBAB0A0-A21E-4CCD-980E-539376061F81}" name="Timezone" dataDxfId="35"/>
-    <tableColumn id="18" xr3:uid="{1EB4D3C2-CE07-4EA7-B2C8-74185C6E2FEF}" name="Job Priority" dataDxfId="34"/>
-    <tableColumn id="27" xr3:uid="{C533FEE6-8255-4711-A421-D6AB5A91A24C}" name="Items Activation Threshold" dataDxfId="33"/>
-    <tableColumn id="26" xr3:uid="{CC0987F9-E5EB-424C-BAC2-EC7C6CD6AE1A}" name="Items Per Job Activation" dataDxfId="32"/>
-    <tableColumn id="25" xr3:uid="{1AC94E67-3224-488F-8717-86F6A46274E7}" name="Max Jobs For Activation" dataDxfId="31"/>
-    <tableColumn id="23" xr3:uid="{30D62244-4112-4278-BA03-7537ABE2F931}" name="Queue Name" dataDxfId="30"/>
-    <tableColumn id="29" xr3:uid="{6F7B436B-C7DD-40F7-977E-79FB75EAFE78}" name="Calendar Name" dataDxfId="29"/>
-    <tableColumn id="28" xr3:uid="{E0816FFE-1BDE-49AC-A8E8-302C91411073}" name="Runtime Type" dataDxfId="28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:W201" headerRowDxfId="55" dataDxfId="53" totalsRowDxfId="51" headerRowBorderDxfId="54" tableBorderDxfId="52">
+  <autoFilter ref="A1:W201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="23">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Folder ID" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{058B7C0E-F18D-4AA8-A7A4-2A2B65B79498}" name="Folder Name" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{6FFDE20C-2159-4C8B-AE94-46A18EBF32E7}" name="Trigger ID" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{81F71C1A-632D-4A5F-BC94-CC97DF7A65EF}" name="Trigger Name" dataDxfId="47"/>
+    <tableColumn id="17" xr3:uid="{E6C314EE-6A01-4E6A-AF88-E0387E29802E}" name="Enabled" dataDxfId="46"/>
+    <tableColumn id="15" xr3:uid="{2DEE6F64-66B8-46E2-8DED-978C18789A63}" name="Process Name" dataDxfId="45"/>
+    <tableColumn id="14" xr3:uid="{6AFD31D0-7236-4B61-B6F7-B7E209179C91}" name="Input Arguments Definition" dataDxfId="44"/>
+    <tableColumn id="13" xr3:uid="{DB22136F-7CCB-43B3-B2F3-F64F00569B2B}" name="Use Calendar" dataDxfId="43"/>
+    <tableColumn id="12" xr3:uid="{4B4F4CCE-4592-4435-91E9-4E3F0FE0353D}" name="Start Strategy (-1 All Robots;0 Specific Robots;&gt;0 Execute XX times)" dataDxfId="42"/>
+    <tableColumn id="11" xr3:uid="{6382E3E3-5FAD-4667-9BD7-D16BEF5953FF}" name="Start Process Cron" dataDxfId="41"/>
+    <tableColumn id="10" xr3:uid="{7A8F0FC9-8380-4F42-9505-29FB8CBCB859}" name="Start Process Cron Details" dataDxfId="40"/>
+    <tableColumn id="9" xr3:uid="{AF0F06BF-7B1B-43E6-A374-D2A97BE7CA57}" name="Stop Strategy" dataDxfId="39"/>
+    <tableColumn id="22" xr3:uid="{E47DF96B-8D93-4081-8137-B872BBA545F0}" name="Stop Process Date" dataDxfId="38"/>
+    <tableColumn id="21" xr3:uid="{5505F1C6-570D-45E3-9390-0F6EFEE4654C}" name="Stop Process Expression" dataDxfId="37"/>
+    <tableColumn id="20" xr3:uid="{5FBAB0A0-A21E-4CCD-980E-539376061F81}" name="Timezone" dataDxfId="36"/>
+    <tableColumn id="18" xr3:uid="{1EB4D3C2-CE07-4EA7-B2C8-74185C6E2FEF}" name="Job Priority" dataDxfId="35"/>
+    <tableColumn id="27" xr3:uid="{C533FEE6-8255-4711-A421-D6AB5A91A24C}" name="Items Activation Threshold" dataDxfId="34"/>
+    <tableColumn id="26" xr3:uid="{CC0987F9-E5EB-424C-BAC2-EC7C6CD6AE1A}" name="Items Per Job Activation" dataDxfId="33"/>
+    <tableColumn id="25" xr3:uid="{1AC94E67-3224-488F-8717-86F6A46274E7}" name="Max Jobs For Activation" dataDxfId="32"/>
+    <tableColumn id="23" xr3:uid="{30D62244-4112-4278-BA03-7537ABE2F931}" name="Queue Name" dataDxfId="31"/>
+    <tableColumn id="29" xr3:uid="{6F7B436B-C7DD-40F7-977E-79FB75EAFE78}" name="Calendar Name" dataDxfId="30"/>
+    <tableColumn id="28" xr3:uid="{E0816FFE-1BDE-49AC-A8E8-302C91411073}" name="Runtime Type" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{60143A08-4321-4F41-AD94-A28222A4F811}" name="Specified Robot ID's" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1785,29 +1816,29 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:W201" totalsRowShown="0">
   <autoFilter ref="A1:W201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="23">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Folder Name" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{3F114B58-2997-4D73-A80A-40D21B742757}" name="Trigger Name" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{45B7C249-3DF1-450D-AA47-E72B0FE30A90}" name="Enabled" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{FD574CB7-FA08-4654-9CD7-86D60F34DB32}" name="Process Name" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{7446F334-E6E0-4A0E-8EB5-68FB9D43F164}" name="Input Arguments Definition" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{9112BA16-F1A6-4B5B-9292-E1F862C46582}" name="Use Calendar" dataDxfId="22"/>
-    <tableColumn id="17" xr3:uid="{EDBD2CF6-8937-4430-880E-CBC035D999B9}" name="Start Strategy (Execute XX times)" dataDxfId="21"/>
-    <tableColumn id="16" xr3:uid="{17E46FA8-B1FA-4C01-B909-101B4EBE2771}" name="Start Process Cron" dataDxfId="20"/>
-    <tableColumn id="15" xr3:uid="{C32A3E10-03CD-4CDE-862C-B8BCCE543C7C}" name="Start Process Cron Details" dataDxfId="19"/>
-    <tableColumn id="14" xr3:uid="{DF244F76-D9C5-4B2A-A7FF-45B1E3C0C680}" name="Stop Strategy" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{F8BF873D-C98E-4452-A769-1730BAA59018}" name="Stop Process Date" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{F1B1C282-F479-4190-ADF0-BBDE31D5EFDB}" name="Stop Process Expression" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{670C436B-1C2B-4D6A-86BB-6E37C846E72C}" name="Timezone" dataDxfId="15"/>
-    <tableColumn id="21" xr3:uid="{95C00957-7AEE-4E5A-8494-3D628AFB4D6C}" name="Job Priority" dataDxfId="14"/>
-    <tableColumn id="20" xr3:uid="{CDA69AC6-5479-479E-B18C-36DFF3254945}" name="Items Activation Threshold" dataDxfId="13"/>
-    <tableColumn id="19" xr3:uid="{8E859498-36EB-4FDD-AAD6-41CC93FE4779}" name="Items Per Job Activation Target" dataDxfId="12"/>
-    <tableColumn id="18" xr3:uid="{08F82746-079C-4356-9DB9-1968920B347F}" name="Max Jobs For Activation" dataDxfId="11"/>
-    <tableColumn id="25" xr3:uid="{3EFAE5F4-8E3E-477D-95CB-475B3BAF404F}" name="Queue Name" dataDxfId="10"/>
-    <tableColumn id="24" xr3:uid="{FE42FDBB-617A-49AC-9EEA-7F486125AE50}" name="Calendar Name" dataDxfId="9"/>
-    <tableColumn id="23" xr3:uid="{FF130F51-8B1A-4457-8500-568BE985E460}" name="Runtime Type" dataDxfId="8"/>
-    <tableColumn id="1" xr3:uid="{4F583ADB-8987-4584-9B76-C3EFCC339400}" name="Username" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Trigger ID" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="Result" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Folder Name" dataDxfId="28"/>
+    <tableColumn id="9" xr3:uid="{3F114B58-2997-4D73-A80A-40D21B742757}" name="Trigger Name" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{45B7C249-3DF1-450D-AA47-E72B0FE30A90}" name="Enabled" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{FD574CB7-FA08-4654-9CD7-86D60F34DB32}" name="Process Name" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{7446F334-E6E0-4A0E-8EB5-68FB9D43F164}" name="Input Arguments Definition" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{9112BA16-F1A6-4B5B-9292-E1F862C46582}" name="Use Calendar" dataDxfId="23"/>
+    <tableColumn id="17" xr3:uid="{EDBD2CF6-8937-4430-880E-CBC035D999B9}" name="Start Strategy (Execute XX times)" dataDxfId="22"/>
+    <tableColumn id="16" xr3:uid="{17E46FA8-B1FA-4C01-B909-101B4EBE2771}" name="Start Process Cron" dataDxfId="21"/>
+    <tableColumn id="15" xr3:uid="{C32A3E10-03CD-4CDE-862C-B8BCCE543C7C}" name="Start Process Cron Details" dataDxfId="20"/>
+    <tableColumn id="14" xr3:uid="{DF244F76-D9C5-4B2A-A7FF-45B1E3C0C680}" name="Stop Strategy" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{F8BF873D-C98E-4452-A769-1730BAA59018}" name="Stop Process Date" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{F1B1C282-F479-4190-ADF0-BBDE31D5EFDB}" name="Stop Process Expression" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{670C436B-1C2B-4D6A-86BB-6E37C846E72C}" name="Timezone" dataDxfId="16"/>
+    <tableColumn id="21" xr3:uid="{95C00957-7AEE-4E5A-8494-3D628AFB4D6C}" name="Job Priority" dataDxfId="15"/>
+    <tableColumn id="20" xr3:uid="{CDA69AC6-5479-479E-B18C-36DFF3254945}" name="Items Activation Threshold" dataDxfId="14"/>
+    <tableColumn id="19" xr3:uid="{8E859498-36EB-4FDD-AAD6-41CC93FE4779}" name="Items Per Job Activation Target" dataDxfId="13"/>
+    <tableColumn id="18" xr3:uid="{08F82746-079C-4356-9DB9-1968920B347F}" name="Max Jobs For Activation" dataDxfId="12"/>
+    <tableColumn id="25" xr3:uid="{3EFAE5F4-8E3E-477D-95CB-475B3BAF404F}" name="Queue Name" dataDxfId="11"/>
+    <tableColumn id="24" xr3:uid="{FE42FDBB-617A-49AC-9EEA-7F486125AE50}" name="Calendar Name" dataDxfId="10"/>
+    <tableColumn id="23" xr3:uid="{FF130F51-8B1A-4457-8500-568BE985E460}" name="Runtime Type" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{4F583ADB-8987-4584-9B76-C3EFCC339400}" name="Username" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Trigger ID" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="Result" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1817,11 +1848,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:E201" totalsRowShown="0">
   <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Folder ID" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{282C1FE1-B7D1-4787-943D-6839B4D2A495}" name="Folder Name" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{708D46EC-46F9-46D3-89F1-FC1EA77B5A97}" name="Trigger ID" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{77482336-B9C3-42EA-B117-2D0B1D764C3A}" name="Trigger Name" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{9F11D09F-EBB8-481F-9883-602BE1C1BEC7}" name="Result" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Folder ID" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{282C1FE1-B7D1-4787-943D-6839B4D2A495}" name="Folder Name" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{708D46EC-46F9-46D3-89F1-FC1EA77B5A97}" name="Trigger ID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{77482336-B9C3-42EA-B117-2D0B1D764C3A}" name="Trigger Name" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{9F11D09F-EBB8-481F-9883-602BE1C1BEC7}" name="Result" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2090,9 +2121,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B90804-4CC2-4F3A-A5A0-B313E9BACDDF}">
-  <dimension ref="A1:V201"/>
+  <dimension ref="A1:W201"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2102,21 +2133,22 @@
     <col min="5" max="5" width="15.75" style="19" customWidth="1"/>
     <col min="6" max="6" width="25.75" customWidth="1"/>
     <col min="7" max="7" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="15.75" customWidth="1"/>
+    <col min="8" max="8" width="15.75" customWidth="1"/>
+    <col min="9" max="9" width="64.58203125" customWidth="1"/>
     <col min="10" max="15" width="25.75" customWidth="1"/>
     <col min="16" max="16" width="15.75" customWidth="1"/>
     <col min="17" max="17" width="27.4140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="25" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="25.75" customWidth="1"/>
+    <col min="20" max="23" width="25.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -2137,49 +2169,52 @@
         <v>6</v>
       </c>
       <c r="I1" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="Q1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="R1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="S1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="T1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="U1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="V1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="21" t="s">
-        <v>20</v>
+      <c r="W1" s="21" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -2202,8 +2237,9 @@
       <c r="T2" s="18"/>
       <c r="U2" s="18"/>
       <c r="V2" s="18"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W2" s="18"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2226,8 +2262,9 @@
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
       <c r="V3" s="18"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W3" s="18"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2250,8 +2287,9 @@
       <c r="T4" s="18"/>
       <c r="U4" s="18"/>
       <c r="V4" s="18"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W4" s="18"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -2274,8 +2312,9 @@
       <c r="T5" s="18"/>
       <c r="U5" s="18"/>
       <c r="V5" s="18"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W5" s="18"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2298,8 +2337,9 @@
       <c r="T6" s="18"/>
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W6" s="18"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -2322,8 +2362,9 @@
       <c r="T7" s="18"/>
       <c r="U7" s="18"/>
       <c r="V7" s="18"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W7" s="18"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -2346,8 +2387,9 @@
       <c r="T8" s="18"/>
       <c r="U8" s="18"/>
       <c r="V8" s="18"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W8" s="18"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2370,8 +2412,9 @@
       <c r="T9" s="18"/>
       <c r="U9" s="18"/>
       <c r="V9" s="18"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W9" s="18"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -2394,8 +2437,9 @@
       <c r="T10" s="18"/>
       <c r="U10" s="18"/>
       <c r="V10" s="18"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W10" s="18"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -2418,8 +2462,9 @@
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W11" s="6"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -2442,8 +2487,9 @@
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W12" s="6"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -2466,8 +2512,9 @@
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W13" s="6"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -2490,8 +2537,9 @@
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W14" s="6"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -2514,8 +2562,9 @@
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W15" s="6"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -2538,8 +2587,9 @@
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W16" s="6"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -2562,8 +2612,9 @@
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W17" s="6"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -2586,8 +2637,9 @@
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W18" s="6"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -2610,8 +2662,9 @@
       <c r="T19" s="6"/>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W19" s="6"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -2634,8 +2687,9 @@
       <c r="T20" s="6"/>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W20" s="6"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -2658,8 +2712,9 @@
       <c r="T21" s="6"/>
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W21" s="6"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -2682,8 +2737,9 @@
       <c r="T22" s="6"/>
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W22" s="6"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -2706,8 +2762,9 @@
       <c r="T23" s="6"/>
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W23" s="6"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -2730,8 +2787,9 @@
       <c r="T24" s="6"/>
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W24" s="6"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -2754,8 +2812,9 @@
       <c r="T25" s="6"/>
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W25" s="6"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -2778,8 +2837,9 @@
       <c r="T26" s="6"/>
       <c r="U26" s="6"/>
       <c r="V26" s="6"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W26" s="6"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -2802,8 +2862,9 @@
       <c r="T27" s="6"/>
       <c r="U27" s="6"/>
       <c r="V27" s="6"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W27" s="6"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -2826,8 +2887,9 @@
       <c r="T28" s="6"/>
       <c r="U28" s="6"/>
       <c r="V28" s="6"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W28" s="6"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="7"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -2850,8 +2912,9 @@
       <c r="T29" s="6"/>
       <c r="U29" s="6"/>
       <c r="V29" s="6"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W29" s="6"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -2874,8 +2937,9 @@
       <c r="T30" s="6"/>
       <c r="U30" s="6"/>
       <c r="V30" s="6"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W30" s="6"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="7"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -2898,8 +2962,9 @@
       <c r="T31" s="6"/>
       <c r="U31" s="6"/>
       <c r="V31" s="6"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W31" s="6"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="7"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -2922,8 +2987,9 @@
       <c r="T32" s="6"/>
       <c r="U32" s="6"/>
       <c r="V32" s="6"/>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W32" s="6"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -2946,8 +3012,9 @@
       <c r="T33" s="6"/>
       <c r="U33" s="6"/>
       <c r="V33" s="6"/>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W33" s="6"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="7"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -2970,8 +3037,9 @@
       <c r="T34" s="6"/>
       <c r="U34" s="6"/>
       <c r="V34" s="6"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W34" s="6"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="7"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -2994,8 +3062,9 @@
       <c r="T35" s="6"/>
       <c r="U35" s="6"/>
       <c r="V35" s="6"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W35" s="6"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="7"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -3018,8 +3087,9 @@
       <c r="T36" s="6"/>
       <c r="U36" s="6"/>
       <c r="V36" s="6"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W36" s="6"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="7"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -3042,8 +3112,9 @@
       <c r="T37" s="6"/>
       <c r="U37" s="6"/>
       <c r="V37" s="6"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W37" s="6"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="7"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -3066,8 +3137,9 @@
       <c r="T38" s="6"/>
       <c r="U38" s="6"/>
       <c r="V38" s="6"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W38" s="6"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="7"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -3090,8 +3162,9 @@
       <c r="T39" s="6"/>
       <c r="U39" s="6"/>
       <c r="V39" s="6"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W39" s="6"/>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="7"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -3114,8 +3187,9 @@
       <c r="T40" s="6"/>
       <c r="U40" s="6"/>
       <c r="V40" s="6"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W40" s="6"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="7"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -3138,8 +3212,9 @@
       <c r="T41" s="6"/>
       <c r="U41" s="6"/>
       <c r="V41" s="6"/>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W41" s="6"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="7"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -3162,8 +3237,9 @@
       <c r="T42" s="6"/>
       <c r="U42" s="6"/>
       <c r="V42" s="6"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W42" s="6"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="7"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -3186,8 +3262,9 @@
       <c r="T43" s="6"/>
       <c r="U43" s="6"/>
       <c r="V43" s="6"/>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W43" s="6"/>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="7"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -3210,8 +3287,9 @@
       <c r="T44" s="6"/>
       <c r="U44" s="6"/>
       <c r="V44" s="6"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W44" s="6"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="7"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -3234,8 +3312,9 @@
       <c r="T45" s="6"/>
       <c r="U45" s="6"/>
       <c r="V45" s="6"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W45" s="6"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="7"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -3258,8 +3337,9 @@
       <c r="T46" s="6"/>
       <c r="U46" s="6"/>
       <c r="V46" s="6"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W46" s="6"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="7"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -3282,8 +3362,9 @@
       <c r="T47" s="6"/>
       <c r="U47" s="6"/>
       <c r="V47" s="6"/>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W47" s="6"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="7"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -3306,8 +3387,9 @@
       <c r="T48" s="6"/>
       <c r="U48" s="6"/>
       <c r="V48" s="6"/>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W48" s="6"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="7"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -3330,8 +3412,9 @@
       <c r="T49" s="6"/>
       <c r="U49" s="6"/>
       <c r="V49" s="6"/>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W49" s="6"/>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="7"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -3354,8 +3437,9 @@
       <c r="T50" s="6"/>
       <c r="U50" s="6"/>
       <c r="V50" s="6"/>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W50" s="6"/>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="7"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
@@ -3378,8 +3462,9 @@
       <c r="T51" s="6"/>
       <c r="U51" s="6"/>
       <c r="V51" s="6"/>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W51" s="6"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="7"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
@@ -3402,8 +3487,9 @@
       <c r="T52" s="6"/>
       <c r="U52" s="6"/>
       <c r="V52" s="6"/>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W52" s="6"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="7"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -3426,8 +3512,9 @@
       <c r="T53" s="6"/>
       <c r="U53" s="6"/>
       <c r="V53" s="6"/>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W53" s="6"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="7"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
@@ -3450,8 +3537,9 @@
       <c r="T54" s="6"/>
       <c r="U54" s="6"/>
       <c r="V54" s="6"/>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W54" s="6"/>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="7"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
@@ -3474,8 +3562,9 @@
       <c r="T55" s="6"/>
       <c r="U55" s="6"/>
       <c r="V55" s="6"/>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W55" s="6"/>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="7"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
@@ -3498,8 +3587,9 @@
       <c r="T56" s="6"/>
       <c r="U56" s="6"/>
       <c r="V56" s="6"/>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W56" s="6"/>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="7"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -3522,8 +3612,9 @@
       <c r="T57" s="6"/>
       <c r="U57" s="6"/>
       <c r="V57" s="6"/>
-    </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W57" s="6"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="7"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
@@ -3546,8 +3637,9 @@
       <c r="T58" s="6"/>
       <c r="U58" s="6"/>
       <c r="V58" s="6"/>
-    </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W58" s="6"/>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="7"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
@@ -3570,8 +3662,9 @@
       <c r="T59" s="6"/>
       <c r="U59" s="6"/>
       <c r="V59" s="6"/>
-    </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W59" s="6"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="7"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
@@ -3594,8 +3687,9 @@
       <c r="T60" s="6"/>
       <c r="U60" s="6"/>
       <c r="V60" s="6"/>
-    </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W60" s="6"/>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="7"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
@@ -3618,8 +3712,9 @@
       <c r="T61" s="6"/>
       <c r="U61" s="6"/>
       <c r="V61" s="6"/>
-    </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W61" s="6"/>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="7"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -3642,8 +3737,9 @@
       <c r="T62" s="6"/>
       <c r="U62" s="6"/>
       <c r="V62" s="6"/>
-    </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W62" s="6"/>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="7"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
@@ -3666,8 +3762,9 @@
       <c r="T63" s="6"/>
       <c r="U63" s="6"/>
       <c r="V63" s="6"/>
-    </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W63" s="6"/>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="7"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
@@ -3690,8 +3787,9 @@
       <c r="T64" s="6"/>
       <c r="U64" s="6"/>
       <c r="V64" s="6"/>
-    </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W64" s="6"/>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="7"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
@@ -3714,8 +3812,9 @@
       <c r="T65" s="6"/>
       <c r="U65" s="6"/>
       <c r="V65" s="6"/>
-    </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W65" s="6"/>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="7"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
@@ -3738,8 +3837,9 @@
       <c r="T66" s="6"/>
       <c r="U66" s="6"/>
       <c r="V66" s="6"/>
-    </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W66" s="6"/>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="7"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
@@ -3762,8 +3862,9 @@
       <c r="T67" s="6"/>
       <c r="U67" s="6"/>
       <c r="V67" s="6"/>
-    </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W67" s="6"/>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="7"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -3786,8 +3887,9 @@
       <c r="T68" s="6"/>
       <c r="U68" s="6"/>
       <c r="V68" s="6"/>
-    </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W68" s="6"/>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="7"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
@@ -3810,8 +3912,9 @@
       <c r="T69" s="6"/>
       <c r="U69" s="6"/>
       <c r="V69" s="6"/>
-    </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W69" s="6"/>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="7"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
@@ -3834,8 +3937,9 @@
       <c r="T70" s="6"/>
       <c r="U70" s="6"/>
       <c r="V70" s="6"/>
-    </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W70" s="6"/>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="7"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
@@ -3858,8 +3962,9 @@
       <c r="T71" s="6"/>
       <c r="U71" s="6"/>
       <c r="V71" s="6"/>
-    </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W71" s="6"/>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="7"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
@@ -3882,8 +3987,9 @@
       <c r="T72" s="6"/>
       <c r="U72" s="6"/>
       <c r="V72" s="6"/>
-    </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W72" s="6"/>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="7"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
@@ -3906,8 +4012,9 @@
       <c r="T73" s="6"/>
       <c r="U73" s="6"/>
       <c r="V73" s="6"/>
-    </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W73" s="6"/>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="7"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -3930,8 +4037,9 @@
       <c r="T74" s="6"/>
       <c r="U74" s="6"/>
       <c r="V74" s="6"/>
-    </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W74" s="6"/>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="7"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
@@ -3954,8 +4062,9 @@
       <c r="T75" s="6"/>
       <c r="U75" s="6"/>
       <c r="V75" s="6"/>
-    </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W75" s="6"/>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="7"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
@@ -3978,8 +4087,9 @@
       <c r="T76" s="6"/>
       <c r="U76" s="6"/>
       <c r="V76" s="6"/>
-    </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W76" s="6"/>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="7"/>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
@@ -4002,8 +4112,9 @@
       <c r="T77" s="6"/>
       <c r="U77" s="6"/>
       <c r="V77" s="6"/>
-    </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W77" s="6"/>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="7"/>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
@@ -4026,8 +4137,9 @@
       <c r="T78" s="6"/>
       <c r="U78" s="6"/>
       <c r="V78" s="6"/>
-    </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W78" s="6"/>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="7"/>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
@@ -4050,8 +4162,9 @@
       <c r="T79" s="6"/>
       <c r="U79" s="6"/>
       <c r="V79" s="6"/>
-    </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W79" s="6"/>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="7"/>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
@@ -4074,8 +4187,9 @@
       <c r="T80" s="6"/>
       <c r="U80" s="6"/>
       <c r="V80" s="6"/>
-    </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W80" s="6"/>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="7"/>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
@@ -4098,8 +4212,9 @@
       <c r="T81" s="6"/>
       <c r="U81" s="6"/>
       <c r="V81" s="6"/>
-    </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W81" s="6"/>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="7"/>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
@@ -4122,8 +4237,9 @@
       <c r="T82" s="6"/>
       <c r="U82" s="6"/>
       <c r="V82" s="6"/>
-    </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W82" s="6"/>
+    </row>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="7"/>
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
@@ -4146,8 +4262,9 @@
       <c r="T83" s="6"/>
       <c r="U83" s="6"/>
       <c r="V83" s="6"/>
-    </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W83" s="6"/>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="7"/>
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
@@ -4170,8 +4287,9 @@
       <c r="T84" s="6"/>
       <c r="U84" s="6"/>
       <c r="V84" s="6"/>
-    </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W84" s="6"/>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="7"/>
       <c r="B85" s="8"/>
       <c r="C85" s="8"/>
@@ -4194,8 +4312,9 @@
       <c r="T85" s="6"/>
       <c r="U85" s="6"/>
       <c r="V85" s="6"/>
-    </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W85" s="6"/>
+    </row>
+    <row r="86" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="7"/>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
@@ -4218,8 +4337,9 @@
       <c r="T86" s="6"/>
       <c r="U86" s="6"/>
       <c r="V86" s="6"/>
-    </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W86" s="6"/>
+    </row>
+    <row r="87" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="7"/>
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
@@ -4242,8 +4362,9 @@
       <c r="T87" s="6"/>
       <c r="U87" s="6"/>
       <c r="V87" s="6"/>
-    </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W87" s="6"/>
+    </row>
+    <row r="88" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="7"/>
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
@@ -4266,8 +4387,9 @@
       <c r="T88" s="6"/>
       <c r="U88" s="6"/>
       <c r="V88" s="6"/>
-    </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W88" s="6"/>
+    </row>
+    <row r="89" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="7"/>
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
@@ -4290,8 +4412,9 @@
       <c r="T89" s="6"/>
       <c r="U89" s="6"/>
       <c r="V89" s="6"/>
-    </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W89" s="6"/>
+    </row>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="7"/>
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
@@ -4314,8 +4437,9 @@
       <c r="T90" s="6"/>
       <c r="U90" s="6"/>
       <c r="V90" s="6"/>
-    </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W90" s="6"/>
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="7"/>
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
@@ -4338,8 +4462,9 @@
       <c r="T91" s="6"/>
       <c r="U91" s="6"/>
       <c r="V91" s="6"/>
-    </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W91" s="6"/>
+    </row>
+    <row r="92" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="7"/>
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
@@ -4362,8 +4487,9 @@
       <c r="T92" s="6"/>
       <c r="U92" s="6"/>
       <c r="V92" s="6"/>
-    </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W92" s="6"/>
+    </row>
+    <row r="93" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="7"/>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
@@ -4386,8 +4512,9 @@
       <c r="T93" s="6"/>
       <c r="U93" s="6"/>
       <c r="V93" s="6"/>
-    </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W93" s="6"/>
+    </row>
+    <row r="94" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="7"/>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
@@ -4410,8 +4537,9 @@
       <c r="T94" s="6"/>
       <c r="U94" s="6"/>
       <c r="V94" s="6"/>
-    </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W94" s="6"/>
+    </row>
+    <row r="95" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="7"/>
       <c r="B95" s="8"/>
       <c r="C95" s="8"/>
@@ -4434,8 +4562,9 @@
       <c r="T95" s="6"/>
       <c r="U95" s="6"/>
       <c r="V95" s="6"/>
-    </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W95" s="6"/>
+    </row>
+    <row r="96" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="7"/>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
@@ -4458,8 +4587,9 @@
       <c r="T96" s="6"/>
       <c r="U96" s="6"/>
       <c r="V96" s="6"/>
-    </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W96" s="6"/>
+    </row>
+    <row r="97" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="7"/>
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
@@ -4482,8 +4612,9 @@
       <c r="T97" s="6"/>
       <c r="U97" s="6"/>
       <c r="V97" s="6"/>
-    </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W97" s="6"/>
+    </row>
+    <row r="98" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="7"/>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
@@ -4506,8 +4637,9 @@
       <c r="T98" s="6"/>
       <c r="U98" s="6"/>
       <c r="V98" s="6"/>
-    </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W98" s="6"/>
+    </row>
+    <row r="99" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="7"/>
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
@@ -4530,8 +4662,9 @@
       <c r="T99" s="6"/>
       <c r="U99" s="6"/>
       <c r="V99" s="6"/>
-    </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W99" s="6"/>
+    </row>
+    <row r="100" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="7"/>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
@@ -4554,8 +4687,9 @@
       <c r="T100" s="6"/>
       <c r="U100" s="6"/>
       <c r="V100" s="6"/>
-    </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W100" s="6"/>
+    </row>
+    <row r="101" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="9"/>
       <c r="B101" s="10"/>
       <c r="C101" s="10"/>
@@ -4578,8 +4712,9 @@
       <c r="T101" s="22"/>
       <c r="U101" s="22"/>
       <c r="V101" s="22"/>
-    </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W101" s="22"/>
+    </row>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="9"/>
       <c r="B102" s="10"/>
       <c r="C102" s="10"/>
@@ -4602,8 +4737,9 @@
       <c r="T102" s="22"/>
       <c r="U102" s="22"/>
       <c r="V102" s="22"/>
-    </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W102" s="22"/>
+    </row>
+    <row r="103" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="7"/>
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
@@ -4626,8 +4762,9 @@
       <c r="T103" s="6"/>
       <c r="U103" s="6"/>
       <c r="V103" s="6"/>
-    </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W103" s="6"/>
+    </row>
+    <row r="104" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="7"/>
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
@@ -4650,8 +4787,9 @@
       <c r="T104" s="6"/>
       <c r="U104" s="6"/>
       <c r="V104" s="6"/>
-    </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W104" s="6"/>
+    </row>
+    <row r="105" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="7"/>
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
@@ -4674,8 +4812,9 @@
       <c r="T105" s="6"/>
       <c r="U105" s="6"/>
       <c r="V105" s="6"/>
-    </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W105" s="6"/>
+    </row>
+    <row r="106" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="7"/>
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
@@ -4698,8 +4837,9 @@
       <c r="T106" s="6"/>
       <c r="U106" s="6"/>
       <c r="V106" s="6"/>
-    </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W106" s="6"/>
+    </row>
+    <row r="107" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="7"/>
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
@@ -4722,8 +4862,9 @@
       <c r="T107" s="6"/>
       <c r="U107" s="6"/>
       <c r="V107" s="6"/>
-    </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W107" s="6"/>
+    </row>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="7"/>
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
@@ -4746,8 +4887,9 @@
       <c r="T108" s="6"/>
       <c r="U108" s="6"/>
       <c r="V108" s="6"/>
-    </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W108" s="6"/>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="9"/>
       <c r="B109" s="10"/>
       <c r="C109" s="10"/>
@@ -4770,8 +4912,9 @@
       <c r="T109" s="22"/>
       <c r="U109" s="22"/>
       <c r="V109" s="22"/>
-    </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W109" s="22"/>
+    </row>
+    <row r="110" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="7"/>
       <c r="B110" s="8"/>
       <c r="C110" s="8"/>
@@ -4794,8 +4937,9 @@
       <c r="T110" s="6"/>
       <c r="U110" s="6"/>
       <c r="V110" s="6"/>
-    </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W110" s="6"/>
+    </row>
+    <row r="111" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="7"/>
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>
@@ -4818,8 +4962,9 @@
       <c r="T111" s="6"/>
       <c r="U111" s="6"/>
       <c r="V111" s="6"/>
-    </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W111" s="6"/>
+    </row>
+    <row r="112" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="7"/>
       <c r="B112" s="8"/>
       <c r="C112" s="8"/>
@@ -4842,8 +4987,9 @@
       <c r="T112" s="6"/>
       <c r="U112" s="6"/>
       <c r="V112" s="6"/>
-    </row>
-    <row r="113" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W112" s="6"/>
+    </row>
+    <row r="113" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="7"/>
       <c r="B113" s="8"/>
       <c r="C113" s="8"/>
@@ -4866,8 +5012,9 @@
       <c r="T113" s="6"/>
       <c r="U113" s="6"/>
       <c r="V113" s="6"/>
-    </row>
-    <row r="114" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W113" s="6"/>
+    </row>
+    <row r="114" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="7"/>
       <c r="B114" s="8"/>
       <c r="C114" s="8"/>
@@ -4890,8 +5037,9 @@
       <c r="T114" s="6"/>
       <c r="U114" s="6"/>
       <c r="V114" s="6"/>
-    </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W114" s="6"/>
+    </row>
+    <row r="115" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="7"/>
       <c r="B115" s="8"/>
       <c r="C115" s="8"/>
@@ -4914,8 +5062,9 @@
       <c r="T115" s="6"/>
       <c r="U115" s="6"/>
       <c r="V115" s="6"/>
-    </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W115" s="6"/>
+    </row>
+    <row r="116" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="7"/>
       <c r="B116" s="8"/>
       <c r="C116" s="8"/>
@@ -4938,8 +5087,9 @@
       <c r="T116" s="6"/>
       <c r="U116" s="6"/>
       <c r="V116" s="6"/>
-    </row>
-    <row r="117" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W116" s="6"/>
+    </row>
+    <row r="117" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="7"/>
       <c r="B117" s="8"/>
       <c r="C117" s="8"/>
@@ -4962,8 +5112,9 @@
       <c r="T117" s="6"/>
       <c r="U117" s="6"/>
       <c r="V117" s="6"/>
-    </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W117" s="6"/>
+    </row>
+    <row r="118" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="7"/>
       <c r="B118" s="8"/>
       <c r="C118" s="8"/>
@@ -4986,8 +5137,9 @@
       <c r="T118" s="6"/>
       <c r="U118" s="6"/>
       <c r="V118" s="6"/>
-    </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W118" s="6"/>
+    </row>
+    <row r="119" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="7"/>
       <c r="B119" s="8"/>
       <c r="C119" s="8"/>
@@ -5010,8 +5162,9 @@
       <c r="T119" s="6"/>
       <c r="U119" s="6"/>
       <c r="V119" s="6"/>
-    </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W119" s="6"/>
+    </row>
+    <row r="120" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="7"/>
       <c r="B120" s="8"/>
       <c r="C120" s="8"/>
@@ -5034,8 +5187,9 @@
       <c r="T120" s="6"/>
       <c r="U120" s="6"/>
       <c r="V120" s="6"/>
-    </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W120" s="6"/>
+    </row>
+    <row r="121" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="7"/>
       <c r="B121" s="8"/>
       <c r="C121" s="8"/>
@@ -5058,8 +5212,9 @@
       <c r="T121" s="6"/>
       <c r="U121" s="6"/>
       <c r="V121" s="6"/>
-    </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W121" s="6"/>
+    </row>
+    <row r="122" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="7"/>
       <c r="B122" s="8"/>
       <c r="C122" s="8"/>
@@ -5082,8 +5237,9 @@
       <c r="T122" s="6"/>
       <c r="U122" s="6"/>
       <c r="V122" s="6"/>
-    </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W122" s="6"/>
+    </row>
+    <row r="123" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="7"/>
       <c r="B123" s="8"/>
       <c r="C123" s="8"/>
@@ -5106,8 +5262,9 @@
       <c r="T123" s="6"/>
       <c r="U123" s="6"/>
       <c r="V123" s="6"/>
-    </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W123" s="6"/>
+    </row>
+    <row r="124" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="7"/>
       <c r="B124" s="8"/>
       <c r="C124" s="8"/>
@@ -5130,8 +5287,9 @@
       <c r="T124" s="6"/>
       <c r="U124" s="6"/>
       <c r="V124" s="6"/>
-    </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W124" s="6"/>
+    </row>
+    <row r="125" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="7"/>
       <c r="B125" s="8"/>
       <c r="C125" s="8"/>
@@ -5154,8 +5312,9 @@
       <c r="T125" s="6"/>
       <c r="U125" s="6"/>
       <c r="V125" s="6"/>
-    </row>
-    <row r="126" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W125" s="6"/>
+    </row>
+    <row r="126" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="7"/>
       <c r="B126" s="8"/>
       <c r="C126" s="8"/>
@@ -5178,8 +5337,9 @@
       <c r="T126" s="6"/>
       <c r="U126" s="6"/>
       <c r="V126" s="6"/>
-    </row>
-    <row r="127" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W126" s="6"/>
+    </row>
+    <row r="127" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="7"/>
       <c r="B127" s="8"/>
       <c r="C127" s="8"/>
@@ -5202,8 +5362,9 @@
       <c r="T127" s="6"/>
       <c r="U127" s="6"/>
       <c r="V127" s="6"/>
-    </row>
-    <row r="128" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W127" s="6"/>
+    </row>
+    <row r="128" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="7"/>
       <c r="B128" s="8"/>
       <c r="C128" s="8"/>
@@ -5226,8 +5387,9 @@
       <c r="T128" s="6"/>
       <c r="U128" s="6"/>
       <c r="V128" s="6"/>
-    </row>
-    <row r="129" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W128" s="6"/>
+    </row>
+    <row r="129" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="7"/>
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
@@ -5250,8 +5412,9 @@
       <c r="T129" s="6"/>
       <c r="U129" s="6"/>
       <c r="V129" s="6"/>
-    </row>
-    <row r="130" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W129" s="6"/>
+    </row>
+    <row r="130" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="7"/>
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
@@ -5274,8 +5437,9 @@
       <c r="T130" s="6"/>
       <c r="U130" s="6"/>
       <c r="V130" s="6"/>
-    </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W130" s="6"/>
+    </row>
+    <row r="131" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="7"/>
       <c r="B131" s="8"/>
       <c r="C131" s="8"/>
@@ -5298,8 +5462,9 @@
       <c r="T131" s="6"/>
       <c r="U131" s="6"/>
       <c r="V131" s="6"/>
-    </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W131" s="6"/>
+    </row>
+    <row r="132" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="7"/>
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
@@ -5322,8 +5487,9 @@
       <c r="T132" s="6"/>
       <c r="U132" s="6"/>
       <c r="V132" s="6"/>
-    </row>
-    <row r="133" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W132" s="6"/>
+    </row>
+    <row r="133" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="7"/>
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
@@ -5346,8 +5512,9 @@
       <c r="T133" s="6"/>
       <c r="U133" s="6"/>
       <c r="V133" s="6"/>
-    </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W133" s="6"/>
+    </row>
+    <row r="134" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="7"/>
       <c r="B134" s="8"/>
       <c r="C134" s="8"/>
@@ -5370,8 +5537,9 @@
       <c r="T134" s="6"/>
       <c r="U134" s="6"/>
       <c r="V134" s="6"/>
-    </row>
-    <row r="135" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W134" s="6"/>
+    </row>
+    <row r="135" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="7"/>
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
@@ -5394,8 +5562,9 @@
       <c r="T135" s="6"/>
       <c r="U135" s="6"/>
       <c r="V135" s="6"/>
-    </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W135" s="6"/>
+    </row>
+    <row r="136" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="7"/>
       <c r="B136" s="8"/>
       <c r="C136" s="8"/>
@@ -5418,8 +5587,9 @@
       <c r="T136" s="6"/>
       <c r="U136" s="6"/>
       <c r="V136" s="6"/>
-    </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W136" s="6"/>
+    </row>
+    <row r="137" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="7"/>
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
@@ -5442,8 +5612,9 @@
       <c r="T137" s="6"/>
       <c r="U137" s="6"/>
       <c r="V137" s="6"/>
-    </row>
-    <row r="138" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W137" s="6"/>
+    </row>
+    <row r="138" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="7"/>
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
@@ -5466,8 +5637,9 @@
       <c r="T138" s="6"/>
       <c r="U138" s="6"/>
       <c r="V138" s="6"/>
-    </row>
-    <row r="139" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W138" s="6"/>
+    </row>
+    <row r="139" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="7"/>
       <c r="B139" s="8"/>
       <c r="C139" s="8"/>
@@ -5490,8 +5662,9 @@
       <c r="T139" s="6"/>
       <c r="U139" s="6"/>
       <c r="V139" s="6"/>
-    </row>
-    <row r="140" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W139" s="6"/>
+    </row>
+    <row r="140" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="7"/>
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
@@ -5514,8 +5687,9 @@
       <c r="T140" s="6"/>
       <c r="U140" s="6"/>
       <c r="V140" s="6"/>
-    </row>
-    <row r="141" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W140" s="6"/>
+    </row>
+    <row r="141" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="7"/>
       <c r="B141" s="8"/>
       <c r="C141" s="8"/>
@@ -5538,8 +5712,9 @@
       <c r="T141" s="6"/>
       <c r="U141" s="6"/>
       <c r="V141" s="6"/>
-    </row>
-    <row r="142" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W141" s="6"/>
+    </row>
+    <row r="142" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="7"/>
       <c r="B142" s="8"/>
       <c r="C142" s="8"/>
@@ -5562,8 +5737,9 @@
       <c r="T142" s="6"/>
       <c r="U142" s="6"/>
       <c r="V142" s="6"/>
-    </row>
-    <row r="143" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W142" s="6"/>
+    </row>
+    <row r="143" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="7"/>
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
@@ -5586,8 +5762,9 @@
       <c r="T143" s="6"/>
       <c r="U143" s="6"/>
       <c r="V143" s="6"/>
-    </row>
-    <row r="144" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W143" s="6"/>
+    </row>
+    <row r="144" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="7"/>
       <c r="B144" s="8"/>
       <c r="C144" s="8"/>
@@ -5610,8 +5787,9 @@
       <c r="T144" s="6"/>
       <c r="U144" s="6"/>
       <c r="V144" s="6"/>
-    </row>
-    <row r="145" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W144" s="6"/>
+    </row>
+    <row r="145" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="7"/>
       <c r="B145" s="8"/>
       <c r="C145" s="8"/>
@@ -5634,8 +5812,9 @@
       <c r="T145" s="6"/>
       <c r="U145" s="6"/>
       <c r="V145" s="6"/>
-    </row>
-    <row r="146" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W145" s="6"/>
+    </row>
+    <row r="146" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="7"/>
       <c r="B146" s="8"/>
       <c r="C146" s="8"/>
@@ -5658,8 +5837,9 @@
       <c r="T146" s="6"/>
       <c r="U146" s="6"/>
       <c r="V146" s="6"/>
-    </row>
-    <row r="147" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W146" s="6"/>
+    </row>
+    <row r="147" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="7"/>
       <c r="B147" s="8"/>
       <c r="C147" s="8"/>
@@ -5682,8 +5862,9 @@
       <c r="T147" s="6"/>
       <c r="U147" s="6"/>
       <c r="V147" s="6"/>
-    </row>
-    <row r="148" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W147" s="6"/>
+    </row>
+    <row r="148" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="7"/>
       <c r="B148" s="8"/>
       <c r="C148" s="8"/>
@@ -5706,8 +5887,9 @@
       <c r="T148" s="6"/>
       <c r="U148" s="6"/>
       <c r="V148" s="6"/>
-    </row>
-    <row r="149" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W148" s="6"/>
+    </row>
+    <row r="149" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="7"/>
       <c r="B149" s="8"/>
       <c r="C149" s="8"/>
@@ -5730,8 +5912,9 @@
       <c r="T149" s="6"/>
       <c r="U149" s="6"/>
       <c r="V149" s="6"/>
-    </row>
-    <row r="150" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W149" s="6"/>
+    </row>
+    <row r="150" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="7"/>
       <c r="B150" s="8"/>
       <c r="C150" s="8"/>
@@ -5754,8 +5937,9 @@
       <c r="T150" s="6"/>
       <c r="U150" s="6"/>
       <c r="V150" s="6"/>
-    </row>
-    <row r="151" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W150" s="6"/>
+    </row>
+    <row r="151" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="7"/>
       <c r="B151" s="8"/>
       <c r="C151" s="8"/>
@@ -5778,8 +5962,9 @@
       <c r="T151" s="6"/>
       <c r="U151" s="6"/>
       <c r="V151" s="6"/>
-    </row>
-    <row r="152" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W151" s="6"/>
+    </row>
+    <row r="152" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="7"/>
       <c r="B152" s="8"/>
       <c r="C152" s="8"/>
@@ -5802,8 +5987,9 @@
       <c r="T152" s="6"/>
       <c r="U152" s="6"/>
       <c r="V152" s="6"/>
-    </row>
-    <row r="153" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W152" s="6"/>
+    </row>
+    <row r="153" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="7"/>
       <c r="B153" s="8"/>
       <c r="C153" s="8"/>
@@ -5826,8 +6012,9 @@
       <c r="T153" s="6"/>
       <c r="U153" s="6"/>
       <c r="V153" s="6"/>
-    </row>
-    <row r="154" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W153" s="6"/>
+    </row>
+    <row r="154" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="7"/>
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
@@ -5850,8 +6037,9 @@
       <c r="T154" s="6"/>
       <c r="U154" s="6"/>
       <c r="V154" s="6"/>
-    </row>
-    <row r="155" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W154" s="6"/>
+    </row>
+    <row r="155" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="7"/>
       <c r="B155" s="8"/>
       <c r="C155" s="8"/>
@@ -5874,8 +6062,9 @@
       <c r="T155" s="6"/>
       <c r="U155" s="6"/>
       <c r="V155" s="6"/>
-    </row>
-    <row r="156" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W155" s="6"/>
+    </row>
+    <row r="156" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="7"/>
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
@@ -5898,8 +6087,9 @@
       <c r="T156" s="6"/>
       <c r="U156" s="6"/>
       <c r="V156" s="6"/>
-    </row>
-    <row r="157" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W156" s="6"/>
+    </row>
+    <row r="157" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="7"/>
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
@@ -5922,8 +6112,9 @@
       <c r="T157" s="6"/>
       <c r="U157" s="6"/>
       <c r="V157" s="6"/>
-    </row>
-    <row r="158" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W157" s="6"/>
+    </row>
+    <row r="158" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="7"/>
       <c r="B158" s="8"/>
       <c r="C158" s="8"/>
@@ -5946,8 +6137,9 @@
       <c r="T158" s="6"/>
       <c r="U158" s="6"/>
       <c r="V158" s="6"/>
-    </row>
-    <row r="159" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W158" s="6"/>
+    </row>
+    <row r="159" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="7"/>
       <c r="B159" s="8"/>
       <c r="C159" s="8"/>
@@ -5970,8 +6162,9 @@
       <c r="T159" s="6"/>
       <c r="U159" s="6"/>
       <c r="V159" s="6"/>
-    </row>
-    <row r="160" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W159" s="6"/>
+    </row>
+    <row r="160" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="7"/>
       <c r="B160" s="8"/>
       <c r="C160" s="8"/>
@@ -5994,8 +6187,9 @@
       <c r="T160" s="6"/>
       <c r="U160" s="6"/>
       <c r="V160" s="6"/>
-    </row>
-    <row r="161" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W160" s="6"/>
+    </row>
+    <row r="161" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="7"/>
       <c r="B161" s="8"/>
       <c r="C161" s="8"/>
@@ -6018,8 +6212,9 @@
       <c r="T161" s="6"/>
       <c r="U161" s="6"/>
       <c r="V161" s="6"/>
-    </row>
-    <row r="162" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W161" s="6"/>
+    </row>
+    <row r="162" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="7"/>
       <c r="B162" s="8"/>
       <c r="C162" s="8"/>
@@ -6042,8 +6237,9 @@
       <c r="T162" s="6"/>
       <c r="U162" s="6"/>
       <c r="V162" s="6"/>
-    </row>
-    <row r="163" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W162" s="6"/>
+    </row>
+    <row r="163" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="7"/>
       <c r="B163" s="8"/>
       <c r="C163" s="8"/>
@@ -6066,8 +6262,9 @@
       <c r="T163" s="6"/>
       <c r="U163" s="6"/>
       <c r="V163" s="6"/>
-    </row>
-    <row r="164" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W163" s="6"/>
+    </row>
+    <row r="164" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="7"/>
       <c r="B164" s="8"/>
       <c r="C164" s="8"/>
@@ -6090,8 +6287,9 @@
       <c r="T164" s="6"/>
       <c r="U164" s="6"/>
       <c r="V164" s="6"/>
-    </row>
-    <row r="165" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W164" s="6"/>
+    </row>
+    <row r="165" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="7"/>
       <c r="B165" s="8"/>
       <c r="C165" s="8"/>
@@ -6114,8 +6312,9 @@
       <c r="T165" s="6"/>
       <c r="U165" s="6"/>
       <c r="V165" s="6"/>
-    </row>
-    <row r="166" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W165" s="6"/>
+    </row>
+    <row r="166" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="7"/>
       <c r="B166" s="8"/>
       <c r="C166" s="8"/>
@@ -6138,8 +6337,9 @@
       <c r="T166" s="6"/>
       <c r="U166" s="6"/>
       <c r="V166" s="6"/>
-    </row>
-    <row r="167" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W166" s="6"/>
+    </row>
+    <row r="167" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="7"/>
       <c r="B167" s="8"/>
       <c r="C167" s="8"/>
@@ -6162,8 +6362,9 @@
       <c r="T167" s="6"/>
       <c r="U167" s="6"/>
       <c r="V167" s="6"/>
-    </row>
-    <row r="168" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W167" s="6"/>
+    </row>
+    <row r="168" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="7"/>
       <c r="B168" s="8"/>
       <c r="C168" s="8"/>
@@ -6186,8 +6387,9 @@
       <c r="T168" s="6"/>
       <c r="U168" s="6"/>
       <c r="V168" s="6"/>
-    </row>
-    <row r="169" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W168" s="6"/>
+    </row>
+    <row r="169" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="7"/>
       <c r="B169" s="8"/>
       <c r="C169" s="8"/>
@@ -6210,8 +6412,9 @@
       <c r="T169" s="6"/>
       <c r="U169" s="6"/>
       <c r="V169" s="6"/>
-    </row>
-    <row r="170" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W169" s="6"/>
+    </row>
+    <row r="170" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="7"/>
       <c r="B170" s="8"/>
       <c r="C170" s="8"/>
@@ -6234,8 +6437,9 @@
       <c r="T170" s="6"/>
       <c r="U170" s="6"/>
       <c r="V170" s="6"/>
-    </row>
-    <row r="171" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W170" s="6"/>
+    </row>
+    <row r="171" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="7"/>
       <c r="B171" s="8"/>
       <c r="C171" s="8"/>
@@ -6258,8 +6462,9 @@
       <c r="T171" s="6"/>
       <c r="U171" s="6"/>
       <c r="V171" s="6"/>
-    </row>
-    <row r="172" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W171" s="6"/>
+    </row>
+    <row r="172" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="7"/>
       <c r="B172" s="8"/>
       <c r="C172" s="8"/>
@@ -6282,8 +6487,9 @@
       <c r="T172" s="6"/>
       <c r="U172" s="6"/>
       <c r="V172" s="6"/>
-    </row>
-    <row r="173" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W172" s="6"/>
+    </row>
+    <row r="173" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="7"/>
       <c r="B173" s="8"/>
       <c r="C173" s="8"/>
@@ -6306,8 +6512,9 @@
       <c r="T173" s="6"/>
       <c r="U173" s="6"/>
       <c r="V173" s="6"/>
-    </row>
-    <row r="174" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W173" s="6"/>
+    </row>
+    <row r="174" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="7"/>
       <c r="B174" s="8"/>
       <c r="C174" s="8"/>
@@ -6330,8 +6537,9 @@
       <c r="T174" s="6"/>
       <c r="U174" s="6"/>
       <c r="V174" s="6"/>
-    </row>
-    <row r="175" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W174" s="6"/>
+    </row>
+    <row r="175" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="7"/>
       <c r="B175" s="8"/>
       <c r="C175" s="8"/>
@@ -6354,8 +6562,9 @@
       <c r="T175" s="6"/>
       <c r="U175" s="6"/>
       <c r="V175" s="6"/>
-    </row>
-    <row r="176" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W175" s="6"/>
+    </row>
+    <row r="176" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="7"/>
       <c r="B176" s="8"/>
       <c r="C176" s="8"/>
@@ -6378,8 +6587,9 @@
       <c r="T176" s="6"/>
       <c r="U176" s="6"/>
       <c r="V176" s="6"/>
-    </row>
-    <row r="177" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W176" s="6"/>
+    </row>
+    <row r="177" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="7"/>
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
@@ -6402,8 +6612,9 @@
       <c r="T177" s="6"/>
       <c r="U177" s="6"/>
       <c r="V177" s="6"/>
-    </row>
-    <row r="178" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W177" s="6"/>
+    </row>
+    <row r="178" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="7"/>
       <c r="B178" s="8"/>
       <c r="C178" s="8"/>
@@ -6426,8 +6637,9 @@
       <c r="T178" s="6"/>
       <c r="U178" s="6"/>
       <c r="V178" s="6"/>
-    </row>
-    <row r="179" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W178" s="6"/>
+    </row>
+    <row r="179" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="7"/>
       <c r="B179" s="8"/>
       <c r="C179" s="8"/>
@@ -6450,8 +6662,9 @@
       <c r="T179" s="6"/>
       <c r="U179" s="6"/>
       <c r="V179" s="6"/>
-    </row>
-    <row r="180" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W179" s="6"/>
+    </row>
+    <row r="180" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="7"/>
       <c r="B180" s="8"/>
       <c r="C180" s="8"/>
@@ -6474,8 +6687,9 @@
       <c r="T180" s="6"/>
       <c r="U180" s="6"/>
       <c r="V180" s="6"/>
-    </row>
-    <row r="181" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W180" s="6"/>
+    </row>
+    <row r="181" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="7"/>
       <c r="B181" s="8"/>
       <c r="C181" s="8"/>
@@ -6498,8 +6712,9 @@
       <c r="T181" s="6"/>
       <c r="U181" s="6"/>
       <c r="V181" s="6"/>
-    </row>
-    <row r="182" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W181" s="6"/>
+    </row>
+    <row r="182" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="7"/>
       <c r="B182" s="8"/>
       <c r="C182" s="8"/>
@@ -6522,8 +6737,9 @@
       <c r="T182" s="6"/>
       <c r="U182" s="6"/>
       <c r="V182" s="6"/>
-    </row>
-    <row r="183" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W182" s="6"/>
+    </row>
+    <row r="183" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="7"/>
       <c r="B183" s="8"/>
       <c r="C183" s="8"/>
@@ -6546,8 +6762,9 @@
       <c r="T183" s="6"/>
       <c r="U183" s="6"/>
       <c r="V183" s="6"/>
-    </row>
-    <row r="184" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W183" s="6"/>
+    </row>
+    <row r="184" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="7"/>
       <c r="B184" s="8"/>
       <c r="C184" s="8"/>
@@ -6570,8 +6787,9 @@
       <c r="T184" s="6"/>
       <c r="U184" s="6"/>
       <c r="V184" s="6"/>
-    </row>
-    <row r="185" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W184" s="6"/>
+    </row>
+    <row r="185" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="7"/>
       <c r="B185" s="8"/>
       <c r="C185" s="8"/>
@@ -6594,8 +6812,9 @@
       <c r="T185" s="6"/>
       <c r="U185" s="6"/>
       <c r="V185" s="6"/>
-    </row>
-    <row r="186" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W185" s="6"/>
+    </row>
+    <row r="186" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="7"/>
       <c r="B186" s="8"/>
       <c r="C186" s="8"/>
@@ -6618,8 +6837,9 @@
       <c r="T186" s="6"/>
       <c r="U186" s="6"/>
       <c r="V186" s="6"/>
-    </row>
-    <row r="187" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W186" s="6"/>
+    </row>
+    <row r="187" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="7"/>
       <c r="B187" s="8"/>
       <c r="C187" s="8"/>
@@ -6642,8 +6862,9 @@
       <c r="T187" s="6"/>
       <c r="U187" s="6"/>
       <c r="V187" s="6"/>
-    </row>
-    <row r="188" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W187" s="6"/>
+    </row>
+    <row r="188" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="7"/>
       <c r="B188" s="8"/>
       <c r="C188" s="8"/>
@@ -6666,8 +6887,9 @@
       <c r="T188" s="6"/>
       <c r="U188" s="6"/>
       <c r="V188" s="6"/>
-    </row>
-    <row r="189" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W188" s="6"/>
+    </row>
+    <row r="189" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="7"/>
       <c r="B189" s="8"/>
       <c r="C189" s="8"/>
@@ -6690,8 +6912,9 @@
       <c r="T189" s="6"/>
       <c r="U189" s="6"/>
       <c r="V189" s="6"/>
-    </row>
-    <row r="190" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W189" s="6"/>
+    </row>
+    <row r="190" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="7"/>
       <c r="B190" s="8"/>
       <c r="C190" s="8"/>
@@ -6714,8 +6937,9 @@
       <c r="T190" s="6"/>
       <c r="U190" s="6"/>
       <c r="V190" s="6"/>
-    </row>
-    <row r="191" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W190" s="6"/>
+    </row>
+    <row r="191" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="7"/>
       <c r="B191" s="8"/>
       <c r="C191" s="8"/>
@@ -6738,8 +6962,9 @@
       <c r="T191" s="6"/>
       <c r="U191" s="6"/>
       <c r="V191" s="6"/>
-    </row>
-    <row r="192" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W191" s="6"/>
+    </row>
+    <row r="192" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="7"/>
       <c r="B192" s="8"/>
       <c r="C192" s="8"/>
@@ -6762,8 +6987,9 @@
       <c r="T192" s="6"/>
       <c r="U192" s="6"/>
       <c r="V192" s="6"/>
-    </row>
-    <row r="193" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W192" s="6"/>
+    </row>
+    <row r="193" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="7"/>
       <c r="B193" s="8"/>
       <c r="C193" s="8"/>
@@ -6786,8 +7012,9 @@
       <c r="T193" s="6"/>
       <c r="U193" s="6"/>
       <c r="V193" s="6"/>
-    </row>
-    <row r="194" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W193" s="6"/>
+    </row>
+    <row r="194" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="7"/>
       <c r="B194" s="8"/>
       <c r="C194" s="8"/>
@@ -6810,8 +7037,9 @@
       <c r="T194" s="6"/>
       <c r="U194" s="6"/>
       <c r="V194" s="6"/>
-    </row>
-    <row r="195" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W194" s="6"/>
+    </row>
+    <row r="195" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="7"/>
       <c r="B195" s="8"/>
       <c r="C195" s="8"/>
@@ -6834,8 +7062,9 @@
       <c r="T195" s="6"/>
       <c r="U195" s="6"/>
       <c r="V195" s="6"/>
-    </row>
-    <row r="196" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W195" s="6"/>
+    </row>
+    <row r="196" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="7"/>
       <c r="B196" s="8"/>
       <c r="C196" s="8"/>
@@ -6858,8 +7087,9 @@
       <c r="T196" s="6"/>
       <c r="U196" s="6"/>
       <c r="V196" s="6"/>
-    </row>
-    <row r="197" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W196" s="6"/>
+    </row>
+    <row r="197" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="7"/>
       <c r="B197" s="8"/>
       <c r="C197" s="8"/>
@@ -6882,8 +7112,9 @@
       <c r="T197" s="6"/>
       <c r="U197" s="6"/>
       <c r="V197" s="6"/>
-    </row>
-    <row r="198" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W197" s="6"/>
+    </row>
+    <row r="198" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="7"/>
       <c r="B198" s="8"/>
       <c r="C198" s="8"/>
@@ -6906,8 +7137,9 @@
       <c r="T198" s="6"/>
       <c r="U198" s="6"/>
       <c r="V198" s="6"/>
-    </row>
-    <row r="199" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W198" s="6"/>
+    </row>
+    <row r="199" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="7"/>
       <c r="B199" s="8"/>
       <c r="C199" s="8"/>
@@ -6930,8 +7162,9 @@
       <c r="T199" s="6"/>
       <c r="U199" s="6"/>
       <c r="V199" s="6"/>
-    </row>
-    <row r="200" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W199" s="6"/>
+    </row>
+    <row r="200" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="7"/>
       <c r="B200" s="8"/>
       <c r="C200" s="8"/>
@@ -6954,8 +7187,9 @@
       <c r="T200" s="6"/>
       <c r="U200" s="6"/>
       <c r="V200" s="6"/>
-    </row>
-    <row r="201" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="W200" s="6"/>
+    </row>
+    <row r="201" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="9"/>
       <c r="B201" s="10"/>
       <c r="C201" s="10"/>
@@ -6978,6 +7212,7 @@
       <c r="T201" s="22"/>
       <c r="U201" s="22"/>
       <c r="V201" s="22"/>
+      <c r="W201" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
@@ -7003,7 +7238,7 @@
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Max Jobs For Activation" error="Max Jobs For Activation must be an integer greater than 0." sqref="S2:S1048576" xr:uid="{0CEF292A-4807-4771-9136-4A38E9AB306A}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Runtime Type" error="Please select a supported Runtime Type." sqref="V2:V1048576" xr:uid="{BA3C1366-D2FC-46F2-A910-7055F34C9AC8}">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Runtime Type" error="Please select a supported Runtime Type." sqref="W202:W1048576 V2:V201" xr:uid="{BA3C1366-D2FC-46F2-A910-7055F34C9AC8}">
       <formula1>"NonProduction,Attended,Unattended,Studio,Development,StudioX,Headless,StudioPro,TestAutomation"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7019,8 +7254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -7044,7 +7279,7 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>2</v>
@@ -7062,49 +7297,49 @@
         <v>6</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="13" t="s">
-        <v>15</v>
-      </c>
       <c r="P1" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="13" t="s">
-        <v>20</v>
-      </c>
       <c r="U1" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V1" s="15" t="s">
         <v>1</v>
@@ -12151,10 +12386,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
JP-542: Implement Enable/Disable Trigger
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Triggers.xlsx
+++ b/Workbooks/EN/Triggers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A21964-9FE6-4E2E-9A97-65C71EBA3AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D6789F-BFC5-4CDE-8FE2-45CE0F411A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Get" sheetId="4" r:id="rId1"/>
     <sheet name="Create" sheetId="1" r:id="rId2"/>
     <sheet name="Delete" sheetId="2" r:id="rId3"/>
+    <sheet name="Enable or Disable Triggers" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
   <si>
     <t>Result</t>
   </si>
@@ -119,6 +120,10 @@
   </si>
   <si>
     <t>Specified Robot ID's</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Enable</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -343,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -382,11 +387,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="62">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -395,20 +414,144 @@
           <bgColor theme="2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="0" tint="-0.34998626667073579"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
         <top style="thin">
           <color theme="0" tint="-0.34998626667073579"/>
         </top>
         <bottom style="thin">
           <color theme="0" tint="-0.34998626667073579"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="5"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="5"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="5"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="5"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="5"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="5"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="5"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="5"/>
+        </horizontal>
       </border>
       <protection locked="1" hidden="0"/>
     </dxf>
@@ -1585,6 +1728,31 @@
         <left style="thin">
           <color theme="0" tint="-0.34998626667073579"/>
         </left>
+        <right/>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
         <right style="thin">
           <color theme="0" tint="-0.34998626667073579"/>
         </right>
@@ -1781,32 +1949,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:W201" headerRowDxfId="55" dataDxfId="53" totalsRowDxfId="51" headerRowBorderDxfId="54" tableBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:W201" headerRowDxfId="61" dataDxfId="59" totalsRowDxfId="57" headerRowBorderDxfId="60" tableBorderDxfId="58">
   <autoFilter ref="A1:W201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="23">
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Folder ID" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{058B7C0E-F18D-4AA8-A7A4-2A2B65B79498}" name="Folder Name" dataDxfId="49"/>
-    <tableColumn id="1" xr3:uid="{6FFDE20C-2159-4C8B-AE94-46A18EBF32E7}" name="Trigger ID" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{81F71C1A-632D-4A5F-BC94-CC97DF7A65EF}" name="Trigger Name" dataDxfId="47"/>
-    <tableColumn id="17" xr3:uid="{E6C314EE-6A01-4E6A-AF88-E0387E29802E}" name="Enabled" dataDxfId="46"/>
-    <tableColumn id="15" xr3:uid="{2DEE6F64-66B8-46E2-8DED-978C18789A63}" name="Process Name" dataDxfId="45"/>
-    <tableColumn id="14" xr3:uid="{6AFD31D0-7236-4B61-B6F7-B7E209179C91}" name="Input Arguments Definition" dataDxfId="44"/>
-    <tableColumn id="13" xr3:uid="{DB22136F-7CCB-43B3-B2F3-F64F00569B2B}" name="Use Calendar" dataDxfId="43"/>
-    <tableColumn id="12" xr3:uid="{4B4F4CCE-4592-4435-91E9-4E3F0FE0353D}" name="Start Strategy (-1 All Robots;0 Specific Robots;&gt;0 Execute XX times)" dataDxfId="42"/>
-    <tableColumn id="11" xr3:uid="{6382E3E3-5FAD-4667-9BD7-D16BEF5953FF}" name="Start Process Cron" dataDxfId="41"/>
-    <tableColumn id="10" xr3:uid="{7A8F0FC9-8380-4F42-9505-29FB8CBCB859}" name="Start Process Cron Details" dataDxfId="40"/>
-    <tableColumn id="9" xr3:uid="{AF0F06BF-7B1B-43E6-A374-D2A97BE7CA57}" name="Stop Strategy" dataDxfId="39"/>
-    <tableColumn id="22" xr3:uid="{E47DF96B-8D93-4081-8137-B872BBA545F0}" name="Stop Process Date" dataDxfId="38"/>
-    <tableColumn id="21" xr3:uid="{5505F1C6-570D-45E3-9390-0F6EFEE4654C}" name="Stop Process Expression" dataDxfId="37"/>
-    <tableColumn id="20" xr3:uid="{5FBAB0A0-A21E-4CCD-980E-539376061F81}" name="Timezone" dataDxfId="36"/>
-    <tableColumn id="18" xr3:uid="{1EB4D3C2-CE07-4EA7-B2C8-74185C6E2FEF}" name="Job Priority" dataDxfId="35"/>
-    <tableColumn id="27" xr3:uid="{C533FEE6-8255-4711-A421-D6AB5A91A24C}" name="Items Activation Threshold" dataDxfId="34"/>
-    <tableColumn id="26" xr3:uid="{CC0987F9-E5EB-424C-BAC2-EC7C6CD6AE1A}" name="Items Per Job Activation" dataDxfId="33"/>
-    <tableColumn id="25" xr3:uid="{1AC94E67-3224-488F-8717-86F6A46274E7}" name="Max Jobs For Activation" dataDxfId="32"/>
-    <tableColumn id="23" xr3:uid="{30D62244-4112-4278-BA03-7537ABE2F931}" name="Queue Name" dataDxfId="31"/>
-    <tableColumn id="29" xr3:uid="{6F7B436B-C7DD-40F7-977E-79FB75EAFE78}" name="Calendar Name" dataDxfId="30"/>
-    <tableColumn id="28" xr3:uid="{E0816FFE-1BDE-49AC-A8E8-302C91411073}" name="Runtime Type" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{60143A08-4321-4F41-AD94-A28222A4F811}" name="Specified Robot ID's" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Folder ID" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{058B7C0E-F18D-4AA8-A7A4-2A2B65B79498}" name="Folder Name" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{6FFDE20C-2159-4C8B-AE94-46A18EBF32E7}" name="Trigger ID" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{81F71C1A-632D-4A5F-BC94-CC97DF7A65EF}" name="Trigger Name" dataDxfId="53"/>
+    <tableColumn id="17" xr3:uid="{E6C314EE-6A01-4E6A-AF88-E0387E29802E}" name="Enabled" dataDxfId="52"/>
+    <tableColumn id="15" xr3:uid="{2DEE6F64-66B8-46E2-8DED-978C18789A63}" name="Process Name" dataDxfId="51"/>
+    <tableColumn id="14" xr3:uid="{6AFD31D0-7236-4B61-B6F7-B7E209179C91}" name="Input Arguments Definition" dataDxfId="50"/>
+    <tableColumn id="13" xr3:uid="{DB22136F-7CCB-43B3-B2F3-F64F00569B2B}" name="Use Calendar" dataDxfId="49"/>
+    <tableColumn id="12" xr3:uid="{4B4F4CCE-4592-4435-91E9-4E3F0FE0353D}" name="Start Strategy (-1 All Robots;0 Specific Robots;&gt;0 Execute XX times)" dataDxfId="48"/>
+    <tableColumn id="11" xr3:uid="{6382E3E3-5FAD-4667-9BD7-D16BEF5953FF}" name="Start Process Cron" dataDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{7A8F0FC9-8380-4F42-9505-29FB8CBCB859}" name="Start Process Cron Details" dataDxfId="46"/>
+    <tableColumn id="9" xr3:uid="{AF0F06BF-7B1B-43E6-A374-D2A97BE7CA57}" name="Stop Strategy" dataDxfId="45"/>
+    <tableColumn id="22" xr3:uid="{E47DF96B-8D93-4081-8137-B872BBA545F0}" name="Stop Process Date" dataDxfId="44"/>
+    <tableColumn id="21" xr3:uid="{5505F1C6-570D-45E3-9390-0F6EFEE4654C}" name="Stop Process Expression" dataDxfId="43"/>
+    <tableColumn id="20" xr3:uid="{5FBAB0A0-A21E-4CCD-980E-539376061F81}" name="Timezone" dataDxfId="42"/>
+    <tableColumn id="18" xr3:uid="{1EB4D3C2-CE07-4EA7-B2C8-74185C6E2FEF}" name="Job Priority" dataDxfId="41"/>
+    <tableColumn id="27" xr3:uid="{C533FEE6-8255-4711-A421-D6AB5A91A24C}" name="Items Activation Threshold" dataDxfId="40"/>
+    <tableColumn id="26" xr3:uid="{CC0987F9-E5EB-424C-BAC2-EC7C6CD6AE1A}" name="Items Per Job Activation" dataDxfId="39"/>
+    <tableColumn id="25" xr3:uid="{1AC94E67-3224-488F-8717-86F6A46274E7}" name="Max Jobs For Activation" dataDxfId="38"/>
+    <tableColumn id="23" xr3:uid="{30D62244-4112-4278-BA03-7537ABE2F931}" name="Queue Name" dataDxfId="37"/>
+    <tableColumn id="29" xr3:uid="{6F7B436B-C7DD-40F7-977E-79FB75EAFE78}" name="Calendar Name" dataDxfId="36"/>
+    <tableColumn id="28" xr3:uid="{E0816FFE-1BDE-49AC-A8E8-302C91411073}" name="Runtime Type" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{60143A08-4321-4F41-AD94-A28222A4F811}" name="Specified Robot ID's" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1816,29 +1984,29 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:W201" totalsRowShown="0">
   <autoFilter ref="A1:W201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="23">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Folder Name" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{3F114B58-2997-4D73-A80A-40D21B742757}" name="Trigger Name" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{45B7C249-3DF1-450D-AA47-E72B0FE30A90}" name="Enabled" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{FD574CB7-FA08-4654-9CD7-86D60F34DB32}" name="Process Name" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{7446F334-E6E0-4A0E-8EB5-68FB9D43F164}" name="Input Arguments Definition" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{9112BA16-F1A6-4B5B-9292-E1F862C46582}" name="Use Calendar" dataDxfId="23"/>
-    <tableColumn id="17" xr3:uid="{EDBD2CF6-8937-4430-880E-CBC035D999B9}" name="Start Strategy (Execute XX times)" dataDxfId="22"/>
-    <tableColumn id="16" xr3:uid="{17E46FA8-B1FA-4C01-B909-101B4EBE2771}" name="Start Process Cron" dataDxfId="21"/>
-    <tableColumn id="15" xr3:uid="{C32A3E10-03CD-4CDE-862C-B8BCCE543C7C}" name="Start Process Cron Details" dataDxfId="20"/>
-    <tableColumn id="14" xr3:uid="{DF244F76-D9C5-4B2A-A7FF-45B1E3C0C680}" name="Stop Strategy" dataDxfId="19"/>
-    <tableColumn id="13" xr3:uid="{F8BF873D-C98E-4452-A769-1730BAA59018}" name="Stop Process Date" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{F1B1C282-F479-4190-ADF0-BBDE31D5EFDB}" name="Stop Process Expression" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{670C436B-1C2B-4D6A-86BB-6E37C846E72C}" name="Timezone" dataDxfId="16"/>
-    <tableColumn id="21" xr3:uid="{95C00957-7AEE-4E5A-8494-3D628AFB4D6C}" name="Job Priority" dataDxfId="15"/>
-    <tableColumn id="20" xr3:uid="{CDA69AC6-5479-479E-B18C-36DFF3254945}" name="Items Activation Threshold" dataDxfId="14"/>
-    <tableColumn id="19" xr3:uid="{8E859498-36EB-4FDD-AAD6-41CC93FE4779}" name="Items Per Job Activation Target" dataDxfId="13"/>
-    <tableColumn id="18" xr3:uid="{08F82746-079C-4356-9DB9-1968920B347F}" name="Max Jobs For Activation" dataDxfId="12"/>
-    <tableColumn id="25" xr3:uid="{3EFAE5F4-8E3E-477D-95CB-475B3BAF404F}" name="Queue Name" dataDxfId="11"/>
-    <tableColumn id="24" xr3:uid="{FE42FDBB-617A-49AC-9EEA-7F486125AE50}" name="Calendar Name" dataDxfId="10"/>
-    <tableColumn id="23" xr3:uid="{FF130F51-8B1A-4457-8500-568BE985E460}" name="Runtime Type" dataDxfId="9"/>
-    <tableColumn id="1" xr3:uid="{4F583ADB-8987-4584-9B76-C3EFCC339400}" name="Username" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Trigger ID" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="Result" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Folder Name" dataDxfId="33"/>
+    <tableColumn id="9" xr3:uid="{3F114B58-2997-4D73-A80A-40D21B742757}" name="Trigger Name" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{45B7C249-3DF1-450D-AA47-E72B0FE30A90}" name="Enabled" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{FD574CB7-FA08-4654-9CD7-86D60F34DB32}" name="Process Name" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{7446F334-E6E0-4A0E-8EB5-68FB9D43F164}" name="Input Arguments Definition" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{9112BA16-F1A6-4B5B-9292-E1F862C46582}" name="Use Calendar" dataDxfId="28"/>
+    <tableColumn id="17" xr3:uid="{EDBD2CF6-8937-4430-880E-CBC035D999B9}" name="Start Strategy (Execute XX times)" dataDxfId="27"/>
+    <tableColumn id="16" xr3:uid="{17E46FA8-B1FA-4C01-B909-101B4EBE2771}" name="Start Process Cron" dataDxfId="26"/>
+    <tableColumn id="15" xr3:uid="{C32A3E10-03CD-4CDE-862C-B8BCCE543C7C}" name="Start Process Cron Details" dataDxfId="25"/>
+    <tableColumn id="14" xr3:uid="{DF244F76-D9C5-4B2A-A7FF-45B1E3C0C680}" name="Stop Strategy" dataDxfId="24"/>
+    <tableColumn id="13" xr3:uid="{F8BF873D-C98E-4452-A769-1730BAA59018}" name="Stop Process Date" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{F1B1C282-F479-4190-ADF0-BBDE31D5EFDB}" name="Stop Process Expression" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{670C436B-1C2B-4D6A-86BB-6E37C846E72C}" name="Timezone" dataDxfId="21"/>
+    <tableColumn id="21" xr3:uid="{95C00957-7AEE-4E5A-8494-3D628AFB4D6C}" name="Job Priority" dataDxfId="20"/>
+    <tableColumn id="20" xr3:uid="{CDA69AC6-5479-479E-B18C-36DFF3254945}" name="Items Activation Threshold" dataDxfId="19"/>
+    <tableColumn id="19" xr3:uid="{8E859498-36EB-4FDD-AAD6-41CC93FE4779}" name="Items Per Job Activation Target" dataDxfId="18"/>
+    <tableColumn id="18" xr3:uid="{08F82746-079C-4356-9DB9-1968920B347F}" name="Max Jobs For Activation" dataDxfId="17"/>
+    <tableColumn id="25" xr3:uid="{3EFAE5F4-8E3E-477D-95CB-475B3BAF404F}" name="Queue Name" dataDxfId="16"/>
+    <tableColumn id="24" xr3:uid="{FE42FDBB-617A-49AC-9EEA-7F486125AE50}" name="Calendar Name" dataDxfId="15"/>
+    <tableColumn id="23" xr3:uid="{FF130F51-8B1A-4457-8500-568BE985E460}" name="Runtime Type" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{4F583ADB-8987-4584-9B76-C3EFCC339400}" name="Username" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Trigger ID" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="Result" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1848,11 +2016,26 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:E201" totalsRowShown="0">
   <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Folder ID" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{282C1FE1-B7D1-4787-943D-6839B4D2A495}" name="Folder Name" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{708D46EC-46F9-46D3-89F1-FC1EA77B5A97}" name="Trigger ID" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{77482336-B9C3-42EA-B117-2D0B1D764C3A}" name="Trigger Name" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{9F11D09F-EBB8-481F-9883-602BE1C1BEC7}" name="Result" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Folder ID" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{282C1FE1-B7D1-4787-943D-6839B4D2A495}" name="Folder Name" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{708D46EC-46F9-46D3-89F1-FC1EA77B5A97}" name="Trigger ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{77482336-B9C3-42EA-B117-2D0B1D764C3A}" name="Trigger Name" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{9F11D09F-EBB8-481F-9883-602BE1C1BEC7}" name="Result" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C3580A6A-14E1-4092-82D1-121B927E4E49}" name="Table135" displayName="Table135" ref="A1:F201" totalsRowShown="0">
+  <autoFilter ref="A1:F201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{A5F43B15-9E40-491F-B42D-C1B1719E9748}" name="Folder ID" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{40B27D82-75E9-4F85-8481-08EB5A0183AC}" name="Folder Name" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{E2D6965B-9B00-4318-99A6-E3ED4BAF1A55}" name="Trigger ID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{27D0ED0E-0055-46F5-9C83-09DDA7428D74}" name="Trigger Name" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{F54FDE94-27E2-49AE-9656-0D7EF9959301}" name="Enable" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{41B743E0-D3DE-495A-98EF-EFB19CB8E5CA}" name="Result" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13817,4 +14000,1660 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFECC00B-E5DB-4622-9D96-CF281EC479A0}">
+  <dimension ref="A1:F201"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="3" width="25.75" style="1" customWidth="1"/>
+    <col min="4" max="5" width="25.75" customWidth="1"/>
+    <col min="6" max="6" width="45.75" style="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="11"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="11"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="11"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="11"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="11"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="11"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="11"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="5"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="11"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="5"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="11"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="5"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="11"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="11"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="11"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="11"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="5"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="11"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="11"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="23"/>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="11"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="11"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="11"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="11"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="11"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="11"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="11"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="11"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="11"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="11"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="23"/>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="11"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="11"/>
+      <c r="B79" s="11"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="23"/>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="11"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="11"/>
+      <c r="B81" s="11"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="23"/>
+      <c r="F81" s="5"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="11"/>
+      <c r="B82" s="11"/>
+      <c r="C82" s="11"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="5"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="11"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="23"/>
+      <c r="F83" s="5"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="11"/>
+      <c r="B84" s="11"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="23"/>
+      <c r="F84" s="5"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="11"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="23"/>
+      <c r="F85" s="5"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="11"/>
+      <c r="B86" s="11"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="5"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="11"/>
+      <c r="B87" s="11"/>
+      <c r="C87" s="11"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="23"/>
+      <c r="F87" s="5"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" s="11"/>
+      <c r="B88" s="11"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="23"/>
+      <c r="F88" s="5"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="11"/>
+      <c r="B89" s="11"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="5"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="11"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="5"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="11"/>
+      <c r="B91" s="11"/>
+      <c r="C91" s="11"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="5"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="11"/>
+      <c r="B92" s="11"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="5"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="11"/>
+      <c r="B93" s="11"/>
+      <c r="C93" s="11"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="23"/>
+      <c r="F93" s="5"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="11"/>
+      <c r="B94" s="11"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="23"/>
+      <c r="F94" s="5"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="11"/>
+      <c r="B95" s="11"/>
+      <c r="C95" s="11"/>
+      <c r="D95" s="13"/>
+      <c r="E95" s="23"/>
+      <c r="F95" s="5"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="11"/>
+      <c r="B96" s="11"/>
+      <c r="C96" s="11"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="23"/>
+      <c r="F96" s="5"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="11"/>
+      <c r="B97" s="11"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="23"/>
+      <c r="F97" s="5"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="11"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="23"/>
+      <c r="F98" s="5"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="11"/>
+      <c r="B99" s="11"/>
+      <c r="C99" s="11"/>
+      <c r="D99" s="13"/>
+      <c r="E99" s="23"/>
+      <c r="F99" s="5"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="11"/>
+      <c r="B100" s="11"/>
+      <c r="C100" s="11"/>
+      <c r="D100" s="13"/>
+      <c r="E100" s="23"/>
+      <c r="F100" s="5"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="11"/>
+      <c r="B101" s="11"/>
+      <c r="C101" s="11"/>
+      <c r="D101" s="13"/>
+      <c r="E101" s="23"/>
+      <c r="F101" s="5"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="11"/>
+      <c r="B102" s="11"/>
+      <c r="C102" s="11"/>
+      <c r="D102" s="13"/>
+      <c r="E102" s="23"/>
+      <c r="F102" s="5"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="11"/>
+      <c r="B103" s="11"/>
+      <c r="C103" s="11"/>
+      <c r="D103" s="13"/>
+      <c r="E103" s="23"/>
+      <c r="F103" s="5"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="11"/>
+      <c r="B104" s="11"/>
+      <c r="C104" s="11"/>
+      <c r="D104" s="13"/>
+      <c r="E104" s="23"/>
+      <c r="F104" s="5"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" s="11"/>
+      <c r="B105" s="11"/>
+      <c r="C105" s="11"/>
+      <c r="D105" s="13"/>
+      <c r="E105" s="23"/>
+      <c r="F105" s="5"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" s="11"/>
+      <c r="B106" s="11"/>
+      <c r="C106" s="11"/>
+      <c r="D106" s="13"/>
+      <c r="E106" s="23"/>
+      <c r="F106" s="5"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" s="11"/>
+      <c r="B107" s="11"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="23"/>
+      <c r="F107" s="5"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" s="11"/>
+      <c r="B108" s="11"/>
+      <c r="C108" s="11"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="23"/>
+      <c r="F108" s="5"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" s="11"/>
+      <c r="B109" s="11"/>
+      <c r="C109" s="11"/>
+      <c r="D109" s="13"/>
+      <c r="E109" s="23"/>
+      <c r="F109" s="5"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" s="11"/>
+      <c r="B110" s="11"/>
+      <c r="C110" s="11"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="23"/>
+      <c r="F110" s="5"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" s="11"/>
+      <c r="B111" s="11"/>
+      <c r="C111" s="11"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="23"/>
+      <c r="F111" s="5"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" s="11"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="23"/>
+      <c r="F112" s="5"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" s="11"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="23"/>
+      <c r="F113" s="5"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" s="11"/>
+      <c r="B114" s="11"/>
+      <c r="C114" s="11"/>
+      <c r="D114" s="13"/>
+      <c r="E114" s="23"/>
+      <c r="F114" s="5"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" s="11"/>
+      <c r="B115" s="11"/>
+      <c r="C115" s="11"/>
+      <c r="D115" s="13"/>
+      <c r="E115" s="23"/>
+      <c r="F115" s="5"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" s="11"/>
+      <c r="B116" s="11"/>
+      <c r="C116" s="11"/>
+      <c r="D116" s="13"/>
+      <c r="E116" s="23"/>
+      <c r="F116" s="5"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" s="11"/>
+      <c r="B117" s="11"/>
+      <c r="C117" s="11"/>
+      <c r="D117" s="13"/>
+      <c r="E117" s="23"/>
+      <c r="F117" s="5"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" s="11"/>
+      <c r="B118" s="11"/>
+      <c r="C118" s="11"/>
+      <c r="D118" s="13"/>
+      <c r="E118" s="23"/>
+      <c r="F118" s="5"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" s="11"/>
+      <c r="B119" s="11"/>
+      <c r="C119" s="11"/>
+      <c r="D119" s="13"/>
+      <c r="E119" s="23"/>
+      <c r="F119" s="5"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" s="11"/>
+      <c r="B120" s="11"/>
+      <c r="C120" s="11"/>
+      <c r="D120" s="13"/>
+      <c r="E120" s="23"/>
+      <c r="F120" s="5"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121" s="11"/>
+      <c r="B121" s="11"/>
+      <c r="C121" s="11"/>
+      <c r="D121" s="13"/>
+      <c r="E121" s="23"/>
+      <c r="F121" s="5"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" s="11"/>
+      <c r="B122" s="11"/>
+      <c r="C122" s="11"/>
+      <c r="D122" s="13"/>
+      <c r="E122" s="23"/>
+      <c r="F122" s="5"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123" s="11"/>
+      <c r="B123" s="11"/>
+      <c r="C123" s="11"/>
+      <c r="D123" s="13"/>
+      <c r="E123" s="23"/>
+      <c r="F123" s="5"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" s="11"/>
+      <c r="B124" s="11"/>
+      <c r="C124" s="11"/>
+      <c r="D124" s="13"/>
+      <c r="E124" s="23"/>
+      <c r="F124" s="5"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" s="11"/>
+      <c r="B125" s="11"/>
+      <c r="C125" s="11"/>
+      <c r="D125" s="13"/>
+      <c r="E125" s="23"/>
+      <c r="F125" s="5"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" s="11"/>
+      <c r="B126" s="11"/>
+      <c r="C126" s="11"/>
+      <c r="D126" s="13"/>
+      <c r="E126" s="23"/>
+      <c r="F126" s="5"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" s="11"/>
+      <c r="B127" s="11"/>
+      <c r="C127" s="11"/>
+      <c r="D127" s="13"/>
+      <c r="E127" s="23"/>
+      <c r="F127" s="5"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" s="11"/>
+      <c r="B128" s="11"/>
+      <c r="C128" s="11"/>
+      <c r="D128" s="13"/>
+      <c r="E128" s="23"/>
+      <c r="F128" s="5"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" s="11"/>
+      <c r="B129" s="11"/>
+      <c r="C129" s="11"/>
+      <c r="D129" s="13"/>
+      <c r="E129" s="23"/>
+      <c r="F129" s="5"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130" s="11"/>
+      <c r="B130" s="11"/>
+      <c r="C130" s="11"/>
+      <c r="D130" s="13"/>
+      <c r="E130" s="23"/>
+      <c r="F130" s="5"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" s="11"/>
+      <c r="B131" s="11"/>
+      <c r="C131" s="11"/>
+      <c r="D131" s="13"/>
+      <c r="E131" s="23"/>
+      <c r="F131" s="5"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" s="11"/>
+      <c r="B132" s="11"/>
+      <c r="C132" s="11"/>
+      <c r="D132" s="13"/>
+      <c r="E132" s="23"/>
+      <c r="F132" s="5"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" s="11"/>
+      <c r="B133" s="11"/>
+      <c r="C133" s="11"/>
+      <c r="D133" s="13"/>
+      <c r="E133" s="23"/>
+      <c r="F133" s="5"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" s="11"/>
+      <c r="B134" s="11"/>
+      <c r="C134" s="11"/>
+      <c r="D134" s="13"/>
+      <c r="E134" s="23"/>
+      <c r="F134" s="5"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" s="11"/>
+      <c r="B135" s="11"/>
+      <c r="C135" s="11"/>
+      <c r="D135" s="13"/>
+      <c r="E135" s="23"/>
+      <c r="F135" s="5"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136" s="11"/>
+      <c r="B136" s="11"/>
+      <c r="C136" s="11"/>
+      <c r="D136" s="13"/>
+      <c r="E136" s="23"/>
+      <c r="F136" s="5"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137" s="11"/>
+      <c r="B137" s="11"/>
+      <c r="C137" s="11"/>
+      <c r="D137" s="13"/>
+      <c r="E137" s="23"/>
+      <c r="F137" s="5"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138" s="11"/>
+      <c r="B138" s="11"/>
+      <c r="C138" s="11"/>
+      <c r="D138" s="13"/>
+      <c r="E138" s="23"/>
+      <c r="F138" s="5"/>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139" s="11"/>
+      <c r="B139" s="11"/>
+      <c r="C139" s="11"/>
+      <c r="D139" s="13"/>
+      <c r="E139" s="23"/>
+      <c r="F139" s="5"/>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140" s="11"/>
+      <c r="B140" s="11"/>
+      <c r="C140" s="11"/>
+      <c r="D140" s="13"/>
+      <c r="E140" s="23"/>
+      <c r="F140" s="5"/>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141" s="11"/>
+      <c r="B141" s="11"/>
+      <c r="C141" s="11"/>
+      <c r="D141" s="13"/>
+      <c r="E141" s="23"/>
+      <c r="F141" s="5"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A142" s="11"/>
+      <c r="B142" s="11"/>
+      <c r="C142" s="11"/>
+      <c r="D142" s="13"/>
+      <c r="E142" s="23"/>
+      <c r="F142" s="5"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A143" s="11"/>
+      <c r="B143" s="11"/>
+      <c r="C143" s="11"/>
+      <c r="D143" s="13"/>
+      <c r="E143" s="23"/>
+      <c r="F143" s="5"/>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144" s="11"/>
+      <c r="B144" s="11"/>
+      <c r="C144" s="11"/>
+      <c r="D144" s="13"/>
+      <c r="E144" s="23"/>
+      <c r="F144" s="5"/>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A145" s="11"/>
+      <c r="B145" s="11"/>
+      <c r="C145" s="11"/>
+      <c r="D145" s="13"/>
+      <c r="E145" s="23"/>
+      <c r="F145" s="5"/>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A146" s="11"/>
+      <c r="B146" s="11"/>
+      <c r="C146" s="11"/>
+      <c r="D146" s="13"/>
+      <c r="E146" s="23"/>
+      <c r="F146" s="5"/>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A147" s="11"/>
+      <c r="B147" s="11"/>
+      <c r="C147" s="11"/>
+      <c r="D147" s="13"/>
+      <c r="E147" s="23"/>
+      <c r="F147" s="5"/>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A148" s="11"/>
+      <c r="B148" s="11"/>
+      <c r="C148" s="11"/>
+      <c r="D148" s="13"/>
+      <c r="E148" s="23"/>
+      <c r="F148" s="5"/>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A149" s="11"/>
+      <c r="B149" s="11"/>
+      <c r="C149" s="11"/>
+      <c r="D149" s="13"/>
+      <c r="E149" s="23"/>
+      <c r="F149" s="5"/>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A150" s="11"/>
+      <c r="B150" s="11"/>
+      <c r="C150" s="11"/>
+      <c r="D150" s="13"/>
+      <c r="E150" s="23"/>
+      <c r="F150" s="5"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A151" s="11"/>
+      <c r="B151" s="11"/>
+      <c r="C151" s="11"/>
+      <c r="D151" s="13"/>
+      <c r="E151" s="23"/>
+      <c r="F151" s="5"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A152" s="11"/>
+      <c r="B152" s="11"/>
+      <c r="C152" s="11"/>
+      <c r="D152" s="13"/>
+      <c r="E152" s="23"/>
+      <c r="F152" s="5"/>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A153" s="11"/>
+      <c r="B153" s="11"/>
+      <c r="C153" s="11"/>
+      <c r="D153" s="13"/>
+      <c r="E153" s="23"/>
+      <c r="F153" s="5"/>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A154" s="11"/>
+      <c r="B154" s="11"/>
+      <c r="C154" s="11"/>
+      <c r="D154" s="13"/>
+      <c r="E154" s="23"/>
+      <c r="F154" s="5"/>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A155" s="11"/>
+      <c r="B155" s="11"/>
+      <c r="C155" s="11"/>
+      <c r="D155" s="13"/>
+      <c r="E155" s="23"/>
+      <c r="F155" s="5"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A156" s="11"/>
+      <c r="B156" s="11"/>
+      <c r="C156" s="11"/>
+      <c r="D156" s="13"/>
+      <c r="E156" s="23"/>
+      <c r="F156" s="5"/>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A157" s="11"/>
+      <c r="B157" s="11"/>
+      <c r="C157" s="11"/>
+      <c r="D157" s="13"/>
+      <c r="E157" s="23"/>
+      <c r="F157" s="5"/>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A158" s="11"/>
+      <c r="B158" s="11"/>
+      <c r="C158" s="11"/>
+      <c r="D158" s="13"/>
+      <c r="E158" s="23"/>
+      <c r="F158" s="5"/>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A159" s="11"/>
+      <c r="B159" s="11"/>
+      <c r="C159" s="11"/>
+      <c r="D159" s="13"/>
+      <c r="E159" s="23"/>
+      <c r="F159" s="5"/>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A160" s="11"/>
+      <c r="B160" s="11"/>
+      <c r="C160" s="11"/>
+      <c r="D160" s="13"/>
+      <c r="E160" s="23"/>
+      <c r="F160" s="5"/>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A161" s="11"/>
+      <c r="B161" s="11"/>
+      <c r="C161" s="11"/>
+      <c r="D161" s="13"/>
+      <c r="E161" s="23"/>
+      <c r="F161" s="5"/>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A162" s="11"/>
+      <c r="B162" s="11"/>
+      <c r="C162" s="11"/>
+      <c r="D162" s="13"/>
+      <c r="E162" s="23"/>
+      <c r="F162" s="5"/>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A163" s="11"/>
+      <c r="B163" s="11"/>
+      <c r="C163" s="11"/>
+      <c r="D163" s="13"/>
+      <c r="E163" s="23"/>
+      <c r="F163" s="5"/>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A164" s="11"/>
+      <c r="B164" s="11"/>
+      <c r="C164" s="11"/>
+      <c r="D164" s="13"/>
+      <c r="E164" s="23"/>
+      <c r="F164" s="5"/>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A165" s="11"/>
+      <c r="B165" s="11"/>
+      <c r="C165" s="11"/>
+      <c r="D165" s="13"/>
+      <c r="E165" s="23"/>
+      <c r="F165" s="5"/>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A166" s="11"/>
+      <c r="B166" s="11"/>
+      <c r="C166" s="11"/>
+      <c r="D166" s="13"/>
+      <c r="E166" s="23"/>
+      <c r="F166" s="5"/>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A167" s="11"/>
+      <c r="B167" s="11"/>
+      <c r="C167" s="11"/>
+      <c r="D167" s="13"/>
+      <c r="E167" s="23"/>
+      <c r="F167" s="5"/>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A168" s="11"/>
+      <c r="B168" s="11"/>
+      <c r="C168" s="11"/>
+      <c r="D168" s="13"/>
+      <c r="E168" s="23"/>
+      <c r="F168" s="5"/>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A169" s="11"/>
+      <c r="B169" s="11"/>
+      <c r="C169" s="11"/>
+      <c r="D169" s="13"/>
+      <c r="E169" s="23"/>
+      <c r="F169" s="5"/>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A170" s="11"/>
+      <c r="B170" s="11"/>
+      <c r="C170" s="11"/>
+      <c r="D170" s="13"/>
+      <c r="E170" s="23"/>
+      <c r="F170" s="5"/>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A171" s="11"/>
+      <c r="B171" s="11"/>
+      <c r="C171" s="11"/>
+      <c r="D171" s="13"/>
+      <c r="E171" s="23"/>
+      <c r="F171" s="5"/>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A172" s="11"/>
+      <c r="B172" s="11"/>
+      <c r="C172" s="11"/>
+      <c r="D172" s="13"/>
+      <c r="E172" s="23"/>
+      <c r="F172" s="5"/>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A173" s="11"/>
+      <c r="B173" s="11"/>
+      <c r="C173" s="11"/>
+      <c r="D173" s="13"/>
+      <c r="E173" s="23"/>
+      <c r="F173" s="5"/>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A174" s="11"/>
+      <c r="B174" s="11"/>
+      <c r="C174" s="11"/>
+      <c r="D174" s="13"/>
+      <c r="E174" s="23"/>
+      <c r="F174" s="5"/>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A175" s="11"/>
+      <c r="B175" s="11"/>
+      <c r="C175" s="11"/>
+      <c r="D175" s="13"/>
+      <c r="E175" s="23"/>
+      <c r="F175" s="5"/>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A176" s="11"/>
+      <c r="B176" s="11"/>
+      <c r="C176" s="11"/>
+      <c r="D176" s="13"/>
+      <c r="E176" s="23"/>
+      <c r="F176" s="5"/>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A177" s="11"/>
+      <c r="B177" s="11"/>
+      <c r="C177" s="11"/>
+      <c r="D177" s="13"/>
+      <c r="E177" s="23"/>
+      <c r="F177" s="5"/>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A178" s="11"/>
+      <c r="B178" s="11"/>
+      <c r="C178" s="11"/>
+      <c r="D178" s="13"/>
+      <c r="E178" s="23"/>
+      <c r="F178" s="5"/>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A179" s="11"/>
+      <c r="B179" s="11"/>
+      <c r="C179" s="11"/>
+      <c r="D179" s="13"/>
+      <c r="E179" s="23"/>
+      <c r="F179" s="5"/>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A180" s="11"/>
+      <c r="B180" s="11"/>
+      <c r="C180" s="11"/>
+      <c r="D180" s="13"/>
+      <c r="E180" s="23"/>
+      <c r="F180" s="5"/>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A181" s="11"/>
+      <c r="B181" s="11"/>
+      <c r="C181" s="11"/>
+      <c r="D181" s="13"/>
+      <c r="E181" s="23"/>
+      <c r="F181" s="5"/>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A182" s="11"/>
+      <c r="B182" s="11"/>
+      <c r="C182" s="11"/>
+      <c r="D182" s="13"/>
+      <c r="E182" s="23"/>
+      <c r="F182" s="5"/>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A183" s="11"/>
+      <c r="B183" s="11"/>
+      <c r="C183" s="11"/>
+      <c r="D183" s="13"/>
+      <c r="E183" s="23"/>
+      <c r="F183" s="5"/>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A184" s="11"/>
+      <c r="B184" s="11"/>
+      <c r="C184" s="11"/>
+      <c r="D184" s="13"/>
+      <c r="E184" s="23"/>
+      <c r="F184" s="5"/>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A185" s="11"/>
+      <c r="B185" s="11"/>
+      <c r="C185" s="11"/>
+      <c r="D185" s="13"/>
+      <c r="E185" s="23"/>
+      <c r="F185" s="5"/>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A186" s="11"/>
+      <c r="B186" s="11"/>
+      <c r="C186" s="11"/>
+      <c r="D186" s="13"/>
+      <c r="E186" s="23"/>
+      <c r="F186" s="5"/>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A187" s="11"/>
+      <c r="B187" s="11"/>
+      <c r="C187" s="11"/>
+      <c r="D187" s="13"/>
+      <c r="E187" s="23"/>
+      <c r="F187" s="5"/>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A188" s="11"/>
+      <c r="B188" s="11"/>
+      <c r="C188" s="11"/>
+      <c r="D188" s="13"/>
+      <c r="E188" s="23"/>
+      <c r="F188" s="5"/>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A189" s="11"/>
+      <c r="B189" s="11"/>
+      <c r="C189" s="11"/>
+      <c r="D189" s="13"/>
+      <c r="E189" s="23"/>
+      <c r="F189" s="5"/>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A190" s="11"/>
+      <c r="B190" s="11"/>
+      <c r="C190" s="11"/>
+      <c r="D190" s="13"/>
+      <c r="E190" s="23"/>
+      <c r="F190" s="5"/>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A191" s="11"/>
+      <c r="B191" s="11"/>
+      <c r="C191" s="11"/>
+      <c r="D191" s="13"/>
+      <c r="E191" s="23"/>
+      <c r="F191" s="5"/>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A192" s="11"/>
+      <c r="B192" s="11"/>
+      <c r="C192" s="11"/>
+      <c r="D192" s="13"/>
+      <c r="E192" s="23"/>
+      <c r="F192" s="5"/>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A193" s="11"/>
+      <c r="B193" s="11"/>
+      <c r="C193" s="11"/>
+      <c r="D193" s="13"/>
+      <c r="E193" s="23"/>
+      <c r="F193" s="5"/>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A194" s="11"/>
+      <c r="B194" s="11"/>
+      <c r="C194" s="11"/>
+      <c r="D194" s="13"/>
+      <c r="E194" s="23"/>
+      <c r="F194" s="5"/>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A195" s="11"/>
+      <c r="B195" s="11"/>
+      <c r="C195" s="11"/>
+      <c r="D195" s="13"/>
+      <c r="E195" s="23"/>
+      <c r="F195" s="5"/>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A196" s="11"/>
+      <c r="B196" s="11"/>
+      <c r="C196" s="11"/>
+      <c r="D196" s="13"/>
+      <c r="E196" s="23"/>
+      <c r="F196" s="5"/>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A197" s="11"/>
+      <c r="B197" s="11"/>
+      <c r="C197" s="11"/>
+      <c r="D197" s="13"/>
+      <c r="E197" s="23"/>
+      <c r="F197" s="5"/>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A198" s="11"/>
+      <c r="B198" s="11"/>
+      <c r="C198" s="11"/>
+      <c r="D198" s="13"/>
+      <c r="E198" s="23"/>
+      <c r="F198" s="5"/>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A199" s="11"/>
+      <c r="B199" s="11"/>
+      <c r="C199" s="11"/>
+      <c r="D199" s="13"/>
+      <c r="E199" s="23"/>
+      <c r="F199" s="5"/>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A200" s="11"/>
+      <c r="B200" s="11"/>
+      <c r="C200" s="11"/>
+      <c r="D200" s="13"/>
+      <c r="E200" s="23"/>
+      <c r="F200" s="5"/>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A201" s="11"/>
+      <c r="B201" s="11"/>
+      <c r="C201" s="11"/>
+      <c r="D201" s="13"/>
+      <c r="E201" s="23"/>
+      <c r="F201" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <dataValidations count="3">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Trigger ID" error="Trigger ID must be an integer greater than 0." sqref="C2:C1048576" xr:uid="{EAE72E05-164B-49CF-8B38-870EF125B963}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Folder ID" error="Folder ID must be an integer greater than 0." sqref="A2:A1048576" xr:uid="{CF71CE1F-70B8-4E89-B55B-0247611B3E4A}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{88AC16E9-4C9D-48EC-887B-6FA51B18A793}">
+      <formula1>"TRUE, FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>